<commit_message>
SE UI Frame Upload
SEはSound内のSEフォルダにバトル用と入力用追加
UI Frameはmenu_UIを追加
</commit_message>
<xml_diff>
--- a/Godlibrary/BackLog.xlsx
+++ b/Godlibrary/BackLog.xlsx
@@ -4101,6 +4101,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4143,10 +4147,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -4154,574 +4154,7 @@
     <cellStyle name="標準_チーム編成_スプリントバックログ（第４）" xfId="2"/>
     <cellStyle name="標準_バグシート" xfId="3"/>
   </cellStyles>
-  <dxfs count="813">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
+  <dxfs count="732">
     <dxf>
       <font>
         <condense val="0"/>
@@ -5352,6 +4785,48 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color indexed="22"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="22"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color indexed="55"/>
       </font>
     </dxf>
@@ -6248,6 +5723,27 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color indexed="22"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color indexed="55"/>
       </font>
     </dxf>
@@ -7227,48 +6723,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color indexed="55"/>
       </font>
     </dxf>
@@ -7292,27 +6746,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="22"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -10611,7 +10044,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -10731,7 +10163,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -10851,7 +10282,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -10964,7 +10394,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -15528,53 +14957,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="8" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="99" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="99" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="99" t="s">
+      <c r="B1" s="100" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="100" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="102" t="s">
+      <c r="E1" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="102" t="s">
+      <c r="F1" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="G1" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="H1" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="99" t="s">
+      <c r="I1" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="97" t="s">
+      <c r="J1" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
     </row>
     <row r="2" spans="1:16" s="8" customFormat="1">
-      <c r="A2" s="99"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="99"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="100"/>
       <c r="J2" s="23" t="s">
         <v>11</v>
       </c>
@@ -15598,15 +15027,15 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="8" customFormat="1">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="99"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="100"/>
       <c r="J3" s="20">
         <f t="shared" ref="J3:P3" si="0">INT(($J$4-(COLUMN()-COLUMN($J4))*($J$4/COUNTA($J$2:$P$2))))</f>
         <v>0</v>
@@ -15637,15 +15066,15 @@
       </c>
     </row>
     <row r="4" spans="1:16" s="8" customFormat="1">
-      <c r="A4" s="99"/>
-      <c r="B4" s="100"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="99"/>
+      <c r="A4" s="100"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="103"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="100"/>
       <c r="J4" s="21">
         <f>SUM(J5:J104)</f>
         <v>0</v>
@@ -19254,57 +18683,57 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <conditionalFormatting sqref="D105:D65536">
-    <cfRule type="expression" dxfId="812" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="731" priority="1" stopIfTrue="1">
       <formula>D105="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="811" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="730" priority="2" stopIfTrue="1">
       <formula>D105="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="810" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="729" priority="3" stopIfTrue="1">
       <formula>OR(D105="終了",D105="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:XFD104">
-    <cfRule type="expression" dxfId="809" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="728" priority="4" stopIfTrue="1">
       <formula>$D5="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="808" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="727" priority="5" stopIfTrue="1">
       <formula>$D5="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="807" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="726" priority="6" stopIfTrue="1">
       <formula>OR($D5="終了",$D5="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B105:B65536">
-    <cfRule type="expression" dxfId="806" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="725" priority="7" stopIfTrue="1">
       <formula>D105="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="805" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="724" priority="8" stopIfTrue="1">
       <formula>D105="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="804" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="723" priority="9" stopIfTrue="1">
       <formula>OR(D105="終了",D105="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105:C65536">
-    <cfRule type="expression" dxfId="803" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="722" priority="10" stopIfTrue="1">
       <formula>D105="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="802" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="721" priority="11" stopIfTrue="1">
       <formula>D105="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="801" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="720" priority="12" stopIfTrue="1">
       <formula>OR(D105="終了",D105="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E105:P65536">
-    <cfRule type="expression" dxfId="800" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="719" priority="13" stopIfTrue="1">
       <formula>$D105="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="799" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="718" priority="14" stopIfTrue="1">
       <formula>$D105="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="798" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="717" priority="15" stopIfTrue="1">
       <formula>OR($D105="終了",$D105="完了")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19321,7 +18750,7 @@
   <dimension ref="A1:V66"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -19349,41 +18778,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="8" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="100" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="99" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="105" t="s">
+      <c r="C1" s="100" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="106" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="99" t="s">
+      <c r="E1" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="102" t="s">
+      <c r="F1" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="H1" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="I1" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="99" t="s">
+      <c r="J1" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="97" t="s">
+      <c r="K1" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="108"/>
-      <c r="M1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="110"/>
       <c r="N1" s="71"/>
       <c r="O1" s="71"/>
       <c r="P1" s="71"/>
@@ -19395,16 +18824,16 @@
       <c r="V1" s="71"/>
     </row>
     <row r="2" spans="1:22" s="8" customFormat="1">
-      <c r="A2" s="99"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="99"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="100"/>
       <c r="K2" s="23" t="s">
         <v>44</v>
       </c>
@@ -19416,16 +18845,16 @@
       </c>
     </row>
     <row r="3" spans="1:22" s="8" customFormat="1">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="99"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="100"/>
       <c r="K3" s="20">
         <f>INT(($K$4-(COLUMN()-COLUMN($K4))*($K$4/COUNTA($K$2:$M$2))))</f>
         <v>65</v>
@@ -19440,16 +18869,16 @@
       </c>
     </row>
     <row r="4" spans="1:22" s="8" customFormat="1">
-      <c r="A4" s="99"/>
-      <c r="B4" s="100"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="99"/>
+      <c r="A4" s="100"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="100"/>
       <c r="K4" s="21">
         <f>SUM(K5:K37)</f>
         <v>65</v>
@@ -21208,860 +20637,860 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <conditionalFormatting sqref="D43:D65414">
-    <cfRule type="expression" dxfId="797" priority="307" stopIfTrue="1">
+    <cfRule type="expression" dxfId="716" priority="307" stopIfTrue="1">
       <formula>D43="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="796" priority="308" stopIfTrue="1">
+    <cfRule type="expression" dxfId="715" priority="308" stopIfTrue="1">
       <formula>D43="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="795" priority="309" stopIfTrue="1">
+    <cfRule type="expression" dxfId="714" priority="309" stopIfTrue="1">
       <formula>OR(D43="終了",D43="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO5:XFD6">
-    <cfRule type="expression" dxfId="794" priority="310" stopIfTrue="1">
+    <cfRule type="expression" dxfId="713" priority="310" stopIfTrue="1">
       <formula>$D5="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="793" priority="311" stopIfTrue="1">
+    <cfRule type="expression" dxfId="712" priority="311" stopIfTrue="1">
       <formula>$D5="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="792" priority="312" stopIfTrue="1">
+    <cfRule type="expression" dxfId="711" priority="312" stopIfTrue="1">
       <formula>OR($D5="終了",$D5="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43:B65414">
-    <cfRule type="expression" dxfId="791" priority="313" stopIfTrue="1">
+    <cfRule type="expression" dxfId="710" priority="313" stopIfTrue="1">
       <formula>D43="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="790" priority="314" stopIfTrue="1">
+    <cfRule type="expression" dxfId="709" priority="314" stopIfTrue="1">
       <formula>D43="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="789" priority="315" stopIfTrue="1">
+    <cfRule type="expression" dxfId="708" priority="315" stopIfTrue="1">
       <formula>OR(D43="終了",D43="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:C65414">
-    <cfRule type="expression" dxfId="788" priority="316" stopIfTrue="1">
+    <cfRule type="expression" dxfId="707" priority="316" stopIfTrue="1">
       <formula>D43="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="787" priority="317" stopIfTrue="1">
+    <cfRule type="expression" dxfId="706" priority="317" stopIfTrue="1">
       <formula>D43="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="786" priority="318" stopIfTrue="1">
+    <cfRule type="expression" dxfId="705" priority="318" stopIfTrue="1">
       <formula>OR(D43="終了",D43="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43:M65414">
-    <cfRule type="expression" dxfId="785" priority="319" stopIfTrue="1">
+    <cfRule type="expression" dxfId="704" priority="319" stopIfTrue="1">
       <formula>$D43="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="784" priority="320" stopIfTrue="1">
+    <cfRule type="expression" dxfId="703" priority="320" stopIfTrue="1">
       <formula>$D43="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="783" priority="321" stopIfTrue="1">
+    <cfRule type="expression" dxfId="702" priority="321" stopIfTrue="1">
       <formula>OR($D43="終了",$D43="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I13 A5:IN6 B33:C33 E33 C7:M7 B14:I14 C15:I15 K20 B8:I9 K8:K15 K16:M19 B16:I20 J8:J20 B27:I31 B34:I40 B21:M26 F41:I42 L8:M14 B10:D11 F10:I11 E10:E13 B32:E32 F32:I33 A7:A42 J27:M42">
-    <cfRule type="expression" dxfId="782" priority="187" stopIfTrue="1">
+    <cfRule type="expression" dxfId="701" priority="187" stopIfTrue="1">
       <formula>$E5="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="781" priority="188" stopIfTrue="1">
+    <cfRule type="expression" dxfId="700" priority="188" stopIfTrue="1">
       <formula>$E5="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="780" priority="189" stopIfTrue="1">
+    <cfRule type="expression" dxfId="699" priority="189" stopIfTrue="1">
       <formula>OR($E5="終了",$E5="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:IN7">
-    <cfRule type="expression" dxfId="779" priority="193" stopIfTrue="1">
+    <cfRule type="expression" dxfId="698" priority="193" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="778" priority="194" stopIfTrue="1">
+    <cfRule type="expression" dxfId="697" priority="194" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="777" priority="195" stopIfTrue="1">
+    <cfRule type="expression" dxfId="696" priority="195" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10:IN11">
-    <cfRule type="expression" dxfId="776" priority="199" stopIfTrue="1">
+    <cfRule type="expression" dxfId="695" priority="199" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="775" priority="200" stopIfTrue="1">
+    <cfRule type="expression" dxfId="694" priority="200" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="774" priority="201" stopIfTrue="1">
+    <cfRule type="expression" dxfId="693" priority="201" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:IN19">
-    <cfRule type="expression" dxfId="773" priority="205" stopIfTrue="1">
+    <cfRule type="expression" dxfId="692" priority="205" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="772" priority="206" stopIfTrue="1">
+    <cfRule type="expression" dxfId="691" priority="206" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="771" priority="207" stopIfTrue="1">
+    <cfRule type="expression" dxfId="690" priority="207" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N25:N26 AA25:IN26">
-    <cfRule type="expression" dxfId="770" priority="217" stopIfTrue="1">
+    <cfRule type="expression" dxfId="689" priority="217" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="769" priority="218" stopIfTrue="1">
+    <cfRule type="expression" dxfId="688" priority="218" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="768" priority="219" stopIfTrue="1">
+    <cfRule type="expression" dxfId="687" priority="219" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N29:IN30 N28 AA28:IN28">
-    <cfRule type="expression" dxfId="767" priority="220" stopIfTrue="1">
+    <cfRule type="expression" dxfId="686" priority="220" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="766" priority="221" stopIfTrue="1">
+    <cfRule type="expression" dxfId="685" priority="221" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="765" priority="222" stopIfTrue="1">
+    <cfRule type="expression" dxfId="684" priority="222" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N32:IN32">
-    <cfRule type="expression" dxfId="764" priority="229" stopIfTrue="1">
+    <cfRule type="expression" dxfId="683" priority="229" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="763" priority="230" stopIfTrue="1">
+    <cfRule type="expression" dxfId="682" priority="230" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="762" priority="231" stopIfTrue="1">
+    <cfRule type="expression" dxfId="681" priority="231" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N65:V65 AC65:IN66 S66:T66">
-    <cfRule type="expression" dxfId="761" priority="238" stopIfTrue="1">
+    <cfRule type="expression" dxfId="680" priority="238" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="760" priority="239" stopIfTrue="1">
+    <cfRule type="expression" dxfId="679" priority="239" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="759" priority="240" stopIfTrue="1">
+    <cfRule type="expression" dxfId="678" priority="240" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N35:N40 Y39:IN40 S35:IH37 U38:IH38">
-    <cfRule type="expression" dxfId="758" priority="241" stopIfTrue="1">
+    <cfRule type="expression" dxfId="677" priority="241" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="757" priority="242" stopIfTrue="1">
+    <cfRule type="expression" dxfId="676" priority="242" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="756" priority="243" stopIfTrue="1">
+    <cfRule type="expression" dxfId="675" priority="243" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N42:N47 U42:IN47 N48:IN49">
-    <cfRule type="expression" dxfId="755" priority="244" stopIfTrue="1">
+    <cfRule type="expression" dxfId="674" priority="244" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="754" priority="245" stopIfTrue="1">
+    <cfRule type="expression" dxfId="673" priority="245" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="753" priority="246" stopIfTrue="1">
+    <cfRule type="expression" dxfId="672" priority="246" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N41 U41:IN41">
-    <cfRule type="expression" dxfId="752" priority="247" stopIfTrue="1">
+    <cfRule type="expression" dxfId="671" priority="247" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="751" priority="248" stopIfTrue="1">
+    <cfRule type="expression" dxfId="670" priority="248" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="750" priority="249" stopIfTrue="1">
+    <cfRule type="expression" dxfId="669" priority="249" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N50:IN52">
-    <cfRule type="expression" dxfId="749" priority="253" stopIfTrue="1">
+    <cfRule type="expression" dxfId="668" priority="253" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="748" priority="254" stopIfTrue="1">
+    <cfRule type="expression" dxfId="667" priority="254" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="747" priority="255" stopIfTrue="1">
+    <cfRule type="expression" dxfId="666" priority="255" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N62:IN64">
-    <cfRule type="expression" dxfId="746" priority="265" stopIfTrue="1">
+    <cfRule type="expression" dxfId="665" priority="265" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="745" priority="266" stopIfTrue="1">
+    <cfRule type="expression" dxfId="664" priority="266" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="744" priority="267" stopIfTrue="1">
+    <cfRule type="expression" dxfId="663" priority="267" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC69:IN69 S69:T69">
-    <cfRule type="expression" dxfId="743" priority="271" stopIfTrue="1">
+    <cfRule type="expression" dxfId="662" priority="271" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="742" priority="272" stopIfTrue="1">
+    <cfRule type="expression" dxfId="661" priority="272" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="741" priority="273" stopIfTrue="1">
+    <cfRule type="expression" dxfId="660" priority="273" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC71:IN71 S71:T71">
-    <cfRule type="expression" dxfId="740" priority="277" stopIfTrue="1">
+    <cfRule type="expression" dxfId="659" priority="277" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="739" priority="278" stopIfTrue="1">
+    <cfRule type="expression" dxfId="658" priority="278" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="738" priority="279" stopIfTrue="1">
+    <cfRule type="expression" dxfId="657" priority="279" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N73:IN73">
-    <cfRule type="expression" dxfId="737" priority="280" stopIfTrue="1">
+    <cfRule type="expression" dxfId="656" priority="280" stopIfTrue="1">
       <formula>$E13="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="736" priority="281" stopIfTrue="1">
+    <cfRule type="expression" dxfId="655" priority="281" stopIfTrue="1">
       <formula>$E13="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="735" priority="282" stopIfTrue="1">
+    <cfRule type="expression" dxfId="654" priority="282" stopIfTrue="1">
       <formula>OR($E13="終了",$E13="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q72:IN72">
-    <cfRule type="expression" dxfId="734" priority="289" stopIfTrue="1">
+    <cfRule type="expression" dxfId="653" priority="289" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="733" priority="290" stopIfTrue="1">
+    <cfRule type="expression" dxfId="652" priority="290" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="732" priority="291" stopIfTrue="1">
+    <cfRule type="expression" dxfId="651" priority="291" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N74:IN76">
-    <cfRule type="expression" dxfId="731" priority="295" stopIfTrue="1">
+    <cfRule type="expression" dxfId="650" priority="295" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="730" priority="296" stopIfTrue="1">
+    <cfRule type="expression" dxfId="649" priority="296" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="729" priority="297" stopIfTrue="1">
+    <cfRule type="expression" dxfId="648" priority="297" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N80:IN80">
-    <cfRule type="expression" dxfId="728" priority="298" stopIfTrue="1">
+    <cfRule type="expression" dxfId="647" priority="298" stopIfTrue="1">
       <formula>$E21="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="727" priority="299" stopIfTrue="1">
+    <cfRule type="expression" dxfId="646" priority="299" stopIfTrue="1">
       <formula>$E21="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="726" priority="300" stopIfTrue="1">
+    <cfRule type="expression" dxfId="645" priority="300" stopIfTrue="1">
       <formula>OR($E21="終了",$E21="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81:IN83">
-    <cfRule type="expression" dxfId="725" priority="304" stopIfTrue="1">
+    <cfRule type="expression" dxfId="644" priority="304" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="724" priority="305" stopIfTrue="1">
+    <cfRule type="expression" dxfId="643" priority="305" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="723" priority="306" stopIfTrue="1">
+    <cfRule type="expression" dxfId="642" priority="306" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="722" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="641" priority="67" stopIfTrue="1">
       <formula>$E33="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="721" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="640" priority="68" stopIfTrue="1">
       <formula>$E33="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="720" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="639" priority="69" stopIfTrue="1">
       <formula>OR($E33="終了",$E33="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12:IN12">
-    <cfRule type="expression" dxfId="719" priority="352" stopIfTrue="1">
+    <cfRule type="expression" dxfId="638" priority="352" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="718" priority="353" stopIfTrue="1">
+    <cfRule type="expression" dxfId="637" priority="353" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="717" priority="354" stopIfTrue="1">
+    <cfRule type="expression" dxfId="636" priority="354" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:IN20">
-    <cfRule type="expression" dxfId="716" priority="379" stopIfTrue="1">
+    <cfRule type="expression" dxfId="635" priority="379" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="715" priority="380" stopIfTrue="1">
+    <cfRule type="expression" dxfId="634" priority="380" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="714" priority="381" stopIfTrue="1">
+    <cfRule type="expression" dxfId="633" priority="381" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N78:IN78">
-    <cfRule type="expression" dxfId="713" priority="523" stopIfTrue="1">
+    <cfRule type="expression" dxfId="632" priority="523" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="712" priority="524" stopIfTrue="1">
+    <cfRule type="expression" dxfId="631" priority="524" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="711" priority="525" stopIfTrue="1">
+    <cfRule type="expression" dxfId="630" priority="525" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO18:XFD18">
-    <cfRule type="expression" dxfId="710" priority="1510" stopIfTrue="1">
+    <cfRule type="expression" dxfId="629" priority="1510" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="709" priority="1511" stopIfTrue="1">
+    <cfRule type="expression" dxfId="628" priority="1511" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="708" priority="1512" stopIfTrue="1">
+    <cfRule type="expression" dxfId="627" priority="1512" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N31:IN31">
-    <cfRule type="expression" dxfId="707" priority="1534" stopIfTrue="1">
+    <cfRule type="expression" dxfId="626" priority="1534" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="706" priority="1535" stopIfTrue="1">
+    <cfRule type="expression" dxfId="625" priority="1535" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="705" priority="1536" stopIfTrue="1">
+    <cfRule type="expression" dxfId="624" priority="1536" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N53:IN54">
-    <cfRule type="expression" dxfId="704" priority="1570" stopIfTrue="1">
+    <cfRule type="expression" dxfId="623" priority="1570" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="703" priority="1571" stopIfTrue="1">
+    <cfRule type="expression" dxfId="622" priority="1571" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="702" priority="1572" stopIfTrue="1">
+    <cfRule type="expression" dxfId="621" priority="1572" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO23:XFD26 IO13:XFD14">
-    <cfRule type="expression" dxfId="701" priority="1618" stopIfTrue="1">
+    <cfRule type="expression" dxfId="620" priority="1618" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="700" priority="1619" stopIfTrue="1">
+    <cfRule type="expression" dxfId="619" priority="1619" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="699" priority="1620" stopIfTrue="1">
+    <cfRule type="expression" dxfId="618" priority="1620" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO32:XFD32">
-    <cfRule type="expression" dxfId="698" priority="1801" stopIfTrue="1">
+    <cfRule type="expression" dxfId="617" priority="1801" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="697" priority="1802" stopIfTrue="1">
+    <cfRule type="expression" dxfId="616" priority="1802" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="696" priority="1803" stopIfTrue="1">
+    <cfRule type="expression" dxfId="615" priority="1803" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N60:IN60">
-    <cfRule type="expression" dxfId="695" priority="1816" stopIfTrue="1">
+    <cfRule type="expression" dxfId="614" priority="1816" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="694" priority="1817" stopIfTrue="1">
+    <cfRule type="expression" dxfId="613" priority="1817" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="693" priority="1818" stopIfTrue="1">
+    <cfRule type="expression" dxfId="612" priority="1818" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO46:XFD48">
-    <cfRule type="expression" dxfId="692" priority="1870" stopIfTrue="1">
+    <cfRule type="expression" dxfId="611" priority="1870" stopIfTrue="1">
       <formula>$D16="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="691" priority="1871" stopIfTrue="1">
+    <cfRule type="expression" dxfId="610" priority="1871" stopIfTrue="1">
       <formula>$D16="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="690" priority="1872" stopIfTrue="1">
+    <cfRule type="expression" dxfId="609" priority="1872" stopIfTrue="1">
       <formula>OR($D16="終了",$D16="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO77:XFD77 IO72:XFD72 IO20:XFD20">
-    <cfRule type="expression" dxfId="689" priority="1930" stopIfTrue="1">
+    <cfRule type="expression" dxfId="608" priority="1930" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="688" priority="1931" stopIfTrue="1">
+    <cfRule type="expression" dxfId="607" priority="1931" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="687" priority="1932" stopIfTrue="1">
+    <cfRule type="expression" dxfId="606" priority="1932" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N21:IN21 AA22:IN22 N22">
-    <cfRule type="expression" dxfId="686" priority="2350" stopIfTrue="1">
+    <cfRule type="expression" dxfId="605" priority="2350" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="685" priority="2351" stopIfTrue="1">
+    <cfRule type="expression" dxfId="604" priority="2351" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="684" priority="2352" stopIfTrue="1">
+    <cfRule type="expression" dxfId="603" priority="2352" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S67:T67 AC67:IN67 N61:IN61">
-    <cfRule type="expression" dxfId="683" priority="2446" stopIfTrue="1">
+    <cfRule type="expression" dxfId="602" priority="2446" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="682" priority="2447" stopIfTrue="1">
+    <cfRule type="expression" dxfId="601" priority="2447" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="681" priority="2448" stopIfTrue="1">
+    <cfRule type="expression" dxfId="600" priority="2448" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="II34:XFD34">
-    <cfRule type="expression" dxfId="680" priority="2470" stopIfTrue="1">
+    <cfRule type="expression" dxfId="599" priority="2470" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="679" priority="2471" stopIfTrue="1">
+    <cfRule type="expression" dxfId="598" priority="2471" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="678" priority="2472" stopIfTrue="1">
+    <cfRule type="expression" dxfId="597" priority="2472" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO42:XFD44">
-    <cfRule type="expression" dxfId="677" priority="2518" stopIfTrue="1">
+    <cfRule type="expression" dxfId="596" priority="2518" stopIfTrue="1">
       <formula>$D11="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="676" priority="2519" stopIfTrue="1">
+    <cfRule type="expression" dxfId="595" priority="2519" stopIfTrue="1">
       <formula>$D11="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="675" priority="2520" stopIfTrue="1">
+    <cfRule type="expression" dxfId="594" priority="2520" stopIfTrue="1">
       <formula>OR($D11="終了",$D11="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO41:XFD41">
-    <cfRule type="expression" dxfId="674" priority="2521" stopIfTrue="1">
+    <cfRule type="expression" dxfId="593" priority="2521" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="673" priority="2522" stopIfTrue="1">
+    <cfRule type="expression" dxfId="592" priority="2522" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="672" priority="2523" stopIfTrue="1">
+    <cfRule type="expression" dxfId="591" priority="2523" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D13 F12:H13">
-    <cfRule type="expression" dxfId="671" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="590" priority="13" stopIfTrue="1">
       <formula>$E12="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="670" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="589" priority="14" stopIfTrue="1">
       <formula>$E12="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="669" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="588" priority="15" stopIfTrue="1">
       <formula>OR($E12="終了",$E12="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N55:IN59">
-    <cfRule type="expression" dxfId="668" priority="2701" stopIfTrue="1">
+    <cfRule type="expression" dxfId="587" priority="2701" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="667" priority="2702" stopIfTrue="1">
+    <cfRule type="expression" dxfId="586" priority="2702" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="666" priority="2703" stopIfTrue="1">
+    <cfRule type="expression" dxfId="585" priority="2703" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO27:XFD31">
-    <cfRule type="expression" dxfId="665" priority="2704" stopIfTrue="1">
+    <cfRule type="expression" dxfId="584" priority="2704" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="664" priority="2705" stopIfTrue="1">
+    <cfRule type="expression" dxfId="583" priority="2705" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="663" priority="2706" stopIfTrue="1">
+    <cfRule type="expression" dxfId="582" priority="2706" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO33:XFD33">
-    <cfRule type="expression" dxfId="662" priority="2746" stopIfTrue="1">
+    <cfRule type="expression" dxfId="581" priority="2746" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="661" priority="2747" stopIfTrue="1">
+    <cfRule type="expression" dxfId="580" priority="2747" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="660" priority="2748" stopIfTrue="1">
+    <cfRule type="expression" dxfId="579" priority="2748" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC70:IN70 S70:T70">
-    <cfRule type="expression" dxfId="659" priority="2773" stopIfTrue="1">
+    <cfRule type="expression" dxfId="578" priority="2773" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="658" priority="2774" stopIfTrue="1">
+    <cfRule type="expression" dxfId="577" priority="2774" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="657" priority="2775" stopIfTrue="1">
+    <cfRule type="expression" dxfId="576" priority="2775" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="II35:XFD38">
-    <cfRule type="expression" dxfId="656" priority="2797" stopIfTrue="1">
+    <cfRule type="expression" dxfId="575" priority="2797" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="655" priority="2798" stopIfTrue="1">
+    <cfRule type="expression" dxfId="574" priority="2798" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="654" priority="2799" stopIfTrue="1">
+    <cfRule type="expression" dxfId="573" priority="2799" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO39:XFD39">
-    <cfRule type="expression" dxfId="653" priority="2899" stopIfTrue="1">
+    <cfRule type="expression" dxfId="572" priority="2899" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="652" priority="2900" stopIfTrue="1">
+    <cfRule type="expression" dxfId="571" priority="2900" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="651" priority="2901" stopIfTrue="1">
+    <cfRule type="expression" dxfId="570" priority="2901" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S68:T68 AC68:IN68">
-    <cfRule type="expression" dxfId="650" priority="2929" stopIfTrue="1">
+    <cfRule type="expression" dxfId="569" priority="2929" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="649" priority="2930" stopIfTrue="1">
+    <cfRule type="expression" dxfId="568" priority="2930" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="648" priority="2931" stopIfTrue="1">
+    <cfRule type="expression" dxfId="567" priority="2931" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO40:XFD40 IO54:XFD54">
-    <cfRule type="expression" dxfId="647" priority="2938" stopIfTrue="1">
+    <cfRule type="expression" dxfId="566" priority="2938" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="646" priority="2939" stopIfTrue="1">
+    <cfRule type="expression" dxfId="565" priority="2939" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="645" priority="2940" stopIfTrue="1">
+    <cfRule type="expression" dxfId="564" priority="2940" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO55:XFD55 IO57:XFD59">
-    <cfRule type="expression" dxfId="644" priority="2980" stopIfTrue="1">
+    <cfRule type="expression" dxfId="563" priority="2980" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="643" priority="2981" stopIfTrue="1">
+    <cfRule type="expression" dxfId="562" priority="2981" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="642" priority="2982" stopIfTrue="1">
+    <cfRule type="expression" dxfId="561" priority="2982" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO65:XFD65">
-    <cfRule type="expression" dxfId="641" priority="3010" stopIfTrue="1">
+    <cfRule type="expression" dxfId="560" priority="3010" stopIfTrue="1">
       <formula>$D23="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="640" priority="3011" stopIfTrue="1">
+    <cfRule type="expression" dxfId="559" priority="3011" stopIfTrue="1">
       <formula>$D23="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="639" priority="3012" stopIfTrue="1">
+    <cfRule type="expression" dxfId="558" priority="3012" stopIfTrue="1">
       <formula>OR($D23="終了",$D23="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO61:XFD61">
-    <cfRule type="expression" dxfId="638" priority="3013" stopIfTrue="1">
+    <cfRule type="expression" dxfId="557" priority="3013" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="637" priority="3014" stopIfTrue="1">
+    <cfRule type="expression" dxfId="556" priority="3014" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="636" priority="3015" stopIfTrue="1">
+    <cfRule type="expression" dxfId="555" priority="3015" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="635" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="554" priority="10" stopIfTrue="1">
       <formula>$E7="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="634" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="553" priority="11" stopIfTrue="1">
       <formula>$E7="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="633" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="552" priority="12" stopIfTrue="1">
       <formula>OR($E7="終了",$E7="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N34:IH34">
-    <cfRule type="expression" dxfId="632" priority="3127" stopIfTrue="1">
+    <cfRule type="expression" dxfId="551" priority="3127" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="631" priority="3128" stopIfTrue="1">
+    <cfRule type="expression" dxfId="550" priority="3128" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="630" priority="3129" stopIfTrue="1">
+    <cfRule type="expression" dxfId="549" priority="3129" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO21:XFD21">
-    <cfRule type="expression" dxfId="629" priority="3142" stopIfTrue="1">
+    <cfRule type="expression" dxfId="548" priority="3142" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="628" priority="3143" stopIfTrue="1">
+    <cfRule type="expression" dxfId="547" priority="3143" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="627" priority="3144" stopIfTrue="1">
+    <cfRule type="expression" dxfId="546" priority="3144" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO22:XFD22">
-    <cfRule type="expression" dxfId="626" priority="3145" stopIfTrue="1">
+    <cfRule type="expression" dxfId="545" priority="3145" stopIfTrue="1">
       <formula>$D10="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="625" priority="3146" stopIfTrue="1">
+    <cfRule type="expression" dxfId="544" priority="3146" stopIfTrue="1">
       <formula>$D10="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="624" priority="3147" stopIfTrue="1">
+    <cfRule type="expression" dxfId="543" priority="3147" stopIfTrue="1">
       <formula>OR($D10="終了",$D10="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20:M20 L15:M15 N8:IN9">
-    <cfRule type="expression" dxfId="623" priority="3163" stopIfTrue="1">
+    <cfRule type="expression" dxfId="542" priority="3163" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="622" priority="3164" stopIfTrue="1">
+    <cfRule type="expression" dxfId="541" priority="3164" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="621" priority="3165" stopIfTrue="1">
+    <cfRule type="expression" dxfId="540" priority="3165" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N77:IN77">
-    <cfRule type="expression" dxfId="620" priority="3181" stopIfTrue="1">
+    <cfRule type="expression" dxfId="539" priority="3181" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="619" priority="3182" stopIfTrue="1">
+    <cfRule type="expression" dxfId="538" priority="3182" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="618" priority="3183" stopIfTrue="1">
+    <cfRule type="expression" dxfId="537" priority="3183" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO60:XFD60">
-    <cfRule type="expression" dxfId="617" priority="3184" stopIfTrue="1">
+    <cfRule type="expression" dxfId="536" priority="3184" stopIfTrue="1">
       <formula>$D14="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="616" priority="3185" stopIfTrue="1">
+    <cfRule type="expression" dxfId="535" priority="3185" stopIfTrue="1">
       <formula>$D14="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="615" priority="3186" stopIfTrue="1">
+    <cfRule type="expression" dxfId="534" priority="3186" stopIfTrue="1">
       <formula>OR($D14="終了",$D14="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO45:XFD45">
-    <cfRule type="expression" dxfId="614" priority="3190" stopIfTrue="1">
+    <cfRule type="expression" dxfId="533" priority="3190" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="613" priority="3191" stopIfTrue="1">
+    <cfRule type="expression" dxfId="532" priority="3191" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="612" priority="3192" stopIfTrue="1">
+    <cfRule type="expression" dxfId="531" priority="3192" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO50:XFD50">
-    <cfRule type="expression" dxfId="611" priority="3259" stopIfTrue="1">
+    <cfRule type="expression" dxfId="530" priority="3259" stopIfTrue="1">
       <formula>$D21="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="610" priority="3260" stopIfTrue="1">
+    <cfRule type="expression" dxfId="529" priority="3260" stopIfTrue="1">
       <formula>$D21="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="609" priority="3261" stopIfTrue="1">
+    <cfRule type="expression" dxfId="528" priority="3261" stopIfTrue="1">
       <formula>OR($D21="終了",$D21="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="608" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="527" priority="4" stopIfTrue="1">
       <formula>$E15="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="607" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="526" priority="5" stopIfTrue="1">
       <formula>$E15="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="606" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="525" priority="6" stopIfTrue="1">
       <formula>OR($E15="終了",$E15="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO51:XFD52">
-    <cfRule type="expression" dxfId="605" priority="3307" stopIfTrue="1">
+    <cfRule type="expression" dxfId="524" priority="3307" stopIfTrue="1">
       <formula>$D8="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="604" priority="3308" stopIfTrue="1">
+    <cfRule type="expression" dxfId="523" priority="3308" stopIfTrue="1">
       <formula>$D8="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="603" priority="3309" stopIfTrue="1">
+    <cfRule type="expression" dxfId="522" priority="3309" stopIfTrue="1">
       <formula>OR($D8="終了",$D8="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO64:XFD64">
-    <cfRule type="expression" dxfId="602" priority="3352" stopIfTrue="1">
+    <cfRule type="expression" dxfId="521" priority="3352" stopIfTrue="1">
       <formula>$D22="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="601" priority="3353" stopIfTrue="1">
+    <cfRule type="expression" dxfId="520" priority="3353" stopIfTrue="1">
       <formula>$D22="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="600" priority="3354" stopIfTrue="1">
+    <cfRule type="expression" dxfId="519" priority="3354" stopIfTrue="1">
       <formula>OR($D22="終了",$D22="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO76:XFD76">
-    <cfRule type="expression" dxfId="599" priority="3406" stopIfTrue="1">
+    <cfRule type="expression" dxfId="518" priority="3406" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="598" priority="3407" stopIfTrue="1">
+    <cfRule type="expression" dxfId="517" priority="3407" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="597" priority="3408" stopIfTrue="1">
+    <cfRule type="expression" dxfId="516" priority="3408" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO56:XFD56">
-    <cfRule type="expression" dxfId="596" priority="3445" stopIfTrue="1">
+    <cfRule type="expression" dxfId="515" priority="3445" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="595" priority="3446" stopIfTrue="1">
+    <cfRule type="expression" dxfId="514" priority="3446" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="594" priority="3447" stopIfTrue="1">
+    <cfRule type="expression" dxfId="513" priority="3447" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO73:XFD75">
-    <cfRule type="expression" dxfId="593" priority="3478" stopIfTrue="1">
+    <cfRule type="expression" dxfId="512" priority="3478" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="592" priority="3479" stopIfTrue="1">
+    <cfRule type="expression" dxfId="511" priority="3479" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="591" priority="3480" stopIfTrue="1">
+    <cfRule type="expression" dxfId="510" priority="3480" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO66:XFD71">
-    <cfRule type="expression" dxfId="590" priority="3505" stopIfTrue="1">
+    <cfRule type="expression" dxfId="509" priority="3505" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="589" priority="3506" stopIfTrue="1">
+    <cfRule type="expression" dxfId="508" priority="3506" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="588" priority="3507" stopIfTrue="1">
+    <cfRule type="expression" dxfId="507" priority="3507" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27 AA27:IN27">
-    <cfRule type="expression" dxfId="587" priority="3637" stopIfTrue="1">
+    <cfRule type="expression" dxfId="506" priority="3637" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="586" priority="3638" stopIfTrue="1">
+    <cfRule type="expression" dxfId="505" priority="3638" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="585" priority="3639" stopIfTrue="1">
+    <cfRule type="expression" dxfId="504" priority="3639" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13:IN13">
-    <cfRule type="expression" dxfId="584" priority="3643" stopIfTrue="1">
+    <cfRule type="expression" dxfId="503" priority="3643" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="583" priority="3644" stopIfTrue="1">
+    <cfRule type="expression" dxfId="502" priority="3644" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="582" priority="3645" stopIfTrue="1">
+    <cfRule type="expression" dxfId="501" priority="3645" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO7:XFD11">
-    <cfRule type="expression" dxfId="581" priority="3658" stopIfTrue="1">
+    <cfRule type="expression" dxfId="500" priority="3658" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="580" priority="3659" stopIfTrue="1">
+    <cfRule type="expression" dxfId="499" priority="3659" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="579" priority="3660" stopIfTrue="1">
+    <cfRule type="expression" dxfId="498" priority="3660" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA23:IN24 N23:N24">
-    <cfRule type="expression" dxfId="578" priority="3661" stopIfTrue="1">
+    <cfRule type="expression" dxfId="497" priority="3661" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="577" priority="3662" stopIfTrue="1">
+    <cfRule type="expression" dxfId="496" priority="3662" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="576" priority="3663" stopIfTrue="1">
+    <cfRule type="expression" dxfId="495" priority="3663" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO15:XFD17">
-    <cfRule type="expression" dxfId="575" priority="3667" stopIfTrue="1">
+    <cfRule type="expression" dxfId="494" priority="3667" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="574" priority="3668" stopIfTrue="1">
+    <cfRule type="expression" dxfId="493" priority="3668" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="573" priority="3669" stopIfTrue="1">
+    <cfRule type="expression" dxfId="492" priority="3669" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO62:XFD62">
-    <cfRule type="expression" dxfId="572" priority="3706" stopIfTrue="1">
+    <cfRule type="expression" dxfId="491" priority="3706" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="571" priority="3707" stopIfTrue="1">
+    <cfRule type="expression" dxfId="490" priority="3707" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="570" priority="3708" stopIfTrue="1">
+    <cfRule type="expression" dxfId="489" priority="3708" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO63:XFD63">
-    <cfRule type="expression" dxfId="569" priority="3709" stopIfTrue="1">
+    <cfRule type="expression" dxfId="488" priority="3709" stopIfTrue="1">
       <formula>$D19="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="568" priority="3710" stopIfTrue="1">
+    <cfRule type="expression" dxfId="487" priority="3710" stopIfTrue="1">
       <formula>$D19="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="567" priority="3711" stopIfTrue="1">
+    <cfRule type="expression" dxfId="486" priority="3711" stopIfTrue="1">
       <formula>OR($D19="終了",$D19="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41:E42">
-    <cfRule type="expression" dxfId="566" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="485" priority="1" stopIfTrue="1">
       <formula>$E41="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="565" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="484" priority="2" stopIfTrue="1">
       <formula>$E41="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="564" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="483" priority="3" stopIfTrue="1">
       <formula>OR($E41="終了",$E41="完了")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22315,7 +21744,7 @@
   <dimension ref="A1:Y202"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="R134" sqref="R134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -22347,44 +21776,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="8" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="99"/>
-      <c r="B1" s="99" t="s">
+      <c r="A1" s="100"/>
+      <c r="B1" s="100" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="99" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="105" t="s">
+      <c r="C1" s="100" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="106" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="99" t="s">
+      <c r="E1" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="102" t="s">
+      <c r="F1" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="H1" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="I1" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="99" t="s">
+      <c r="J1" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="97" t="s">
+      <c r="K1" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="109"/>
+      <c r="O1" s="109"/>
+      <c r="P1" s="109"/>
+      <c r="Q1" s="109"/>
+      <c r="R1" s="110"/>
       <c r="S1" s="71"/>
       <c r="T1" s="71"/>
       <c r="U1" s="71"/>
@@ -22392,16 +21821,16 @@
       <c r="W1" s="71"/>
     </row>
     <row r="2" spans="1:23" s="8" customFormat="1">
-      <c r="A2" s="99"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="99"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="100"/>
       <c r="K2" s="23" t="s">
         <v>136</v>
       </c>
@@ -22428,16 +21857,16 @@
       </c>
     </row>
     <row r="3" spans="1:23" s="8" customFormat="1">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="99"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="100"/>
       <c r="K3" s="20">
         <f>INT(($K$4-(COLUMN()-COLUMN($K4))*($K$4/COUNTA($K$2:$R$2))))</f>
         <v>173</v>
@@ -22472,22 +21901,22 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="8" customFormat="1">
-      <c r="A4" s="99"/>
-      <c r="B4" s="100"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="99"/>
+      <c r="A4" s="100"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="100"/>
       <c r="K4" s="21">
         <f>SUM(K5:K95)</f>
         <v>173</v>
       </c>
       <c r="L4" s="21">
-        <f t="shared" ref="K4:R4" si="1">SUM(L5:L95)</f>
+        <f t="shared" ref="L4:R4" si="1">SUM(L5:L95)</f>
         <v>160</v>
       </c>
       <c r="M4" s="21">
@@ -24514,7 +23943,7 @@
       </c>
       <c r="V43" s="10">
         <f t="shared" ca="1" si="5"/>
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="W43" s="10">
         <f t="shared" si="6"/>
@@ -24525,7 +23954,7 @@
       </c>
       <c r="Y43" s="15">
         <f t="shared" ca="1" si="7"/>
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:25">
@@ -28796,7 +28225,7 @@
       </c>
       <c r="E129" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>作業中</v>
+        <v>完了</v>
       </c>
       <c r="F129" s="4">
         <v>42740</v>
@@ -28812,7 +28241,7 @@
       </c>
       <c r="J129" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K129" s="22">
         <v>2</v>
@@ -28836,7 +28265,7 @@
         <v>1</v>
       </c>
       <c r="R129" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:18">
@@ -28854,7 +28283,7 @@
       </c>
       <c r="E130" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>作業中</v>
+        <v>完了</v>
       </c>
       <c r="F130" s="4">
         <v>42740</v>
@@ -28870,7 +28299,7 @@
       </c>
       <c r="J130" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K130" s="22">
         <v>2</v>
@@ -28894,7 +28323,7 @@
         <v>1</v>
       </c>
       <c r="R130" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:18">
@@ -28912,7 +28341,7 @@
       </c>
       <c r="E131" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>作業中</v>
+        <v>完了</v>
       </c>
       <c r="F131" s="4">
         <v>42741</v>
@@ -28928,7 +28357,7 @@
       </c>
       <c r="J131" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K131" s="22">
         <v>2</v>
@@ -28952,7 +28381,7 @@
         <v>2</v>
       </c>
       <c r="R131" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:18">
@@ -28970,7 +28399,7 @@
       </c>
       <c r="E132" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>作業中</v>
+        <v>完了</v>
       </c>
       <c r="F132" s="4">
         <v>42741</v>
@@ -28986,7 +28415,7 @@
       </c>
       <c r="J132" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K132" s="22">
         <v>2</v>
@@ -29010,7 +28439,7 @@
         <v>2</v>
       </c>
       <c r="R132" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:18">
@@ -29028,7 +28457,7 @@
       </c>
       <c r="E133" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>作業中</v>
+        <v>完了</v>
       </c>
       <c r="F133" s="4">
         <v>42742</v>
@@ -29044,7 +28473,7 @@
       </c>
       <c r="J133" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K133" s="22">
         <v>2</v>
@@ -29068,7 +28497,7 @@
         <v>2</v>
       </c>
       <c r="R133" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:18">
@@ -31840,783 +31269,783 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <conditionalFormatting sqref="D203:D65439">
-    <cfRule type="expression" dxfId="542" priority="325" stopIfTrue="1">
+    <cfRule type="expression" dxfId="461" priority="325" stopIfTrue="1">
       <formula>D203="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="541" priority="326" stopIfTrue="1">
+    <cfRule type="expression" dxfId="460" priority="326" stopIfTrue="1">
       <formula>D203="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="540" priority="327" stopIfTrue="1">
+    <cfRule type="expression" dxfId="459" priority="327" stopIfTrue="1">
       <formula>OR(D203="終了",D203="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP5:XFD5">
-    <cfRule type="expression" dxfId="539" priority="328" stopIfTrue="1">
+    <cfRule type="expression" dxfId="458" priority="328" stopIfTrue="1">
       <formula>$D5="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="538" priority="329" stopIfTrue="1">
+    <cfRule type="expression" dxfId="457" priority="329" stopIfTrue="1">
       <formula>$D5="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="537" priority="330" stopIfTrue="1">
+    <cfRule type="expression" dxfId="456" priority="330" stopIfTrue="1">
       <formula>OR($D5="終了",$D5="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B203:B65439">
-    <cfRule type="expression" dxfId="536" priority="331" stopIfTrue="1">
+    <cfRule type="expression" dxfId="455" priority="331" stopIfTrue="1">
       <formula>D203="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="535" priority="332" stopIfTrue="1">
+    <cfRule type="expression" dxfId="454" priority="332" stopIfTrue="1">
       <formula>D203="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="534" priority="333" stopIfTrue="1">
+    <cfRule type="expression" dxfId="453" priority="333" stopIfTrue="1">
       <formula>OR(D203="終了",D203="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C203:C65439">
-    <cfRule type="expression" dxfId="533" priority="334" stopIfTrue="1">
+    <cfRule type="expression" dxfId="452" priority="334" stopIfTrue="1">
       <formula>D203="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="532" priority="335" stopIfTrue="1">
+    <cfRule type="expression" dxfId="451" priority="335" stopIfTrue="1">
       <formula>D203="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="531" priority="336" stopIfTrue="1">
+    <cfRule type="expression" dxfId="450" priority="336" stopIfTrue="1">
       <formula>OR(D203="終了",D203="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E203:H65439">
-    <cfRule type="expression" dxfId="530" priority="337" stopIfTrue="1">
+    <cfRule type="expression" dxfId="449" priority="337" stopIfTrue="1">
       <formula>$D203="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="529" priority="338" stopIfTrue="1">
+    <cfRule type="expression" dxfId="448" priority="338" stopIfTrue="1">
       <formula>$D203="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="528" priority="339" stopIfTrue="1">
+    <cfRule type="expression" dxfId="447" priority="339" stopIfTrue="1">
       <formula>OR($D203="終了",$D203="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:IO5 A6:R6 G9:I10 B37:E37 H37 B16:H36 B122:B126 B9:F15 D122:D126 B127:D153 A7:A153 A154:D202 B63:D121 F63:I202 B43:D61 F43:H58 F59:I61 E43:E202 J9:J202 B38:H42 G11:H15 I12:I14 I16:I18 I20:I22 I24:I26 I28:I30 I32:I34 I36:I58 K36:R61 G62 B8:R8 K29:R34 K9:R27 K63:R202">
-    <cfRule type="expression" dxfId="527" priority="205" stopIfTrue="1">
+    <cfRule type="expression" dxfId="446" priority="205" stopIfTrue="1">
       <formula>$E5="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="526" priority="206" stopIfTrue="1">
+    <cfRule type="expression" dxfId="445" priority="206" stopIfTrue="1">
       <formula>$E5="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="525" priority="207" stopIfTrue="1">
+    <cfRule type="expression" dxfId="444" priority="207" stopIfTrue="1">
       <formula>OR($E5="終了",$E5="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C123">
-    <cfRule type="expression" dxfId="524" priority="208" stopIfTrue="1">
+    <cfRule type="expression" dxfId="443" priority="208" stopIfTrue="1">
       <formula>$E122="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="523" priority="209" stopIfTrue="1">
+    <cfRule type="expression" dxfId="442" priority="209" stopIfTrue="1">
       <formula>$E122="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="522" priority="210" stopIfTrue="1">
+    <cfRule type="expression" dxfId="441" priority="210" stopIfTrue="1">
       <formula>OR($E122="終了",$E122="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S6:IO6">
-    <cfRule type="expression" dxfId="521" priority="211" stopIfTrue="1">
+    <cfRule type="expression" dxfId="440" priority="211" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="520" priority="212" stopIfTrue="1">
+    <cfRule type="expression" dxfId="439" priority="212" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="519" priority="213" stopIfTrue="1">
+    <cfRule type="expression" dxfId="438" priority="213" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9:IO10">
-    <cfRule type="expression" dxfId="518" priority="217" stopIfTrue="1">
+    <cfRule type="expression" dxfId="437" priority="217" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="517" priority="218" stopIfTrue="1">
+    <cfRule type="expression" dxfId="436" priority="218" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="516" priority="219" stopIfTrue="1">
+    <cfRule type="expression" dxfId="435" priority="219" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S12:IO16">
-    <cfRule type="expression" dxfId="515" priority="223" stopIfTrue="1">
+    <cfRule type="expression" dxfId="434" priority="223" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="514" priority="224" stopIfTrue="1">
+    <cfRule type="expression" dxfId="433" priority="224" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="513" priority="225" stopIfTrue="1">
+    <cfRule type="expression" dxfId="432" priority="225" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB20:IO20">
-    <cfRule type="expression" dxfId="512" priority="235" stopIfTrue="1">
+    <cfRule type="expression" dxfId="431" priority="235" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="511" priority="236" stopIfTrue="1">
+    <cfRule type="expression" dxfId="430" priority="236" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="510" priority="237" stopIfTrue="1">
+    <cfRule type="expression" dxfId="429" priority="237" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB23:IO23 S24:IO24">
-    <cfRule type="expression" dxfId="509" priority="238" stopIfTrue="1">
+    <cfRule type="expression" dxfId="428" priority="238" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="508" priority="239" stopIfTrue="1">
+    <cfRule type="expression" dxfId="427" priority="239" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="507" priority="240" stopIfTrue="1">
+    <cfRule type="expression" dxfId="426" priority="240" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB21:IO22">
-    <cfRule type="expression" dxfId="506" priority="241" stopIfTrue="1">
+    <cfRule type="expression" dxfId="425" priority="241" stopIfTrue="1">
       <formula>$E15="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="505" priority="242" stopIfTrue="1">
+    <cfRule type="expression" dxfId="424" priority="242" stopIfTrue="1">
       <formula>$E15="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="504" priority="243" stopIfTrue="1">
+    <cfRule type="expression" dxfId="423" priority="243" stopIfTrue="1">
       <formula>OR($E15="終了",$E15="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S26:IO26">
-    <cfRule type="expression" dxfId="503" priority="250" stopIfTrue="1">
+    <cfRule type="expression" dxfId="422" priority="250" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="502" priority="251" stopIfTrue="1">
+    <cfRule type="expression" dxfId="421" priority="251" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="501" priority="252" stopIfTrue="1">
+    <cfRule type="expression" dxfId="420" priority="252" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S44 AD44:IO45">
-    <cfRule type="expression" dxfId="500" priority="256" stopIfTrue="1">
+    <cfRule type="expression" dxfId="419" priority="256" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="499" priority="257" stopIfTrue="1">
+    <cfRule type="expression" dxfId="418" priority="257" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="498" priority="258" stopIfTrue="1">
+    <cfRule type="expression" dxfId="417" priority="258" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S29:S30 Z28:IO30">
-    <cfRule type="expression" dxfId="497" priority="259" stopIfTrue="1">
+    <cfRule type="expression" dxfId="416" priority="259" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="496" priority="260" stopIfTrue="1">
+    <cfRule type="expression" dxfId="415" priority="260" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="495" priority="261" stopIfTrue="1">
+    <cfRule type="expression" dxfId="414" priority="261" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z32:IO33 V30:Y31">
-    <cfRule type="expression" dxfId="494" priority="262" stopIfTrue="1">
+    <cfRule type="expression" dxfId="413" priority="262" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="493" priority="263" stopIfTrue="1">
+    <cfRule type="expression" dxfId="412" priority="263" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="492" priority="264" stopIfTrue="1">
+    <cfRule type="expression" dxfId="411" priority="264" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z31:IO31 V29:Y29">
-    <cfRule type="expression" dxfId="491" priority="265" stopIfTrue="1">
+    <cfRule type="expression" dxfId="410" priority="265" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="490" priority="266" stopIfTrue="1">
+    <cfRule type="expression" dxfId="409" priority="266" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="489" priority="267" stopIfTrue="1">
+    <cfRule type="expression" dxfId="408" priority="267" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S42:S43 Z42:IO43">
-    <cfRule type="expression" dxfId="488" priority="283" stopIfTrue="1">
+    <cfRule type="expression" dxfId="407" priority="283" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="487" priority="284" stopIfTrue="1">
+    <cfRule type="expression" dxfId="406" priority="284" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="486" priority="285" stopIfTrue="1">
+    <cfRule type="expression" dxfId="405" priority="285" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD49:IO49 T47:U47">
-    <cfRule type="expression" dxfId="485" priority="289" stopIfTrue="1">
+    <cfRule type="expression" dxfId="404" priority="289" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="484" priority="290" stopIfTrue="1">
+    <cfRule type="expression" dxfId="403" priority="290" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="483" priority="291" stopIfTrue="1">
+    <cfRule type="expression" dxfId="402" priority="291" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD51:IO51 T49:U49">
-    <cfRule type="expression" dxfId="479" priority="295" stopIfTrue="1">
+    <cfRule type="expression" dxfId="401" priority="295" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="478" priority="296" stopIfTrue="1">
+    <cfRule type="expression" dxfId="400" priority="296" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="477" priority="297" stopIfTrue="1">
+    <cfRule type="expression" dxfId="399" priority="297" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD47:IO47 Z53:IO53 S53">
-    <cfRule type="expression" dxfId="476" priority="298" stopIfTrue="1">
+    <cfRule type="expression" dxfId="398" priority="298" stopIfTrue="1">
       <formula>$E24="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="475" priority="299" stopIfTrue="1">
+    <cfRule type="expression" dxfId="397" priority="299" stopIfTrue="1">
       <formula>$E24="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="474" priority="300" stopIfTrue="1">
+    <cfRule type="expression" dxfId="396" priority="300" stopIfTrue="1">
       <formula>OR($E24="終了",$E24="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S57 Z57:IO57 T55:Y55">
-    <cfRule type="expression" dxfId="473" priority="310" stopIfTrue="1">
+    <cfRule type="expression" dxfId="395" priority="310" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="472" priority="311" stopIfTrue="1">
+    <cfRule type="expression" dxfId="394" priority="311" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="471" priority="312" stopIfTrue="1">
+    <cfRule type="expression" dxfId="393" priority="312" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S54:S56 Z54:IO56 T52:Y54">
-    <cfRule type="expression" dxfId="470" priority="313" stopIfTrue="1">
+    <cfRule type="expression" dxfId="392" priority="313" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="469" priority="314" stopIfTrue="1">
+    <cfRule type="expression" dxfId="391" priority="314" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="468" priority="315" stopIfTrue="1">
+    <cfRule type="expression" dxfId="390" priority="315" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S58:S60 Z58:IO60 T56:Y58">
-    <cfRule type="expression" dxfId="467" priority="316" stopIfTrue="1">
+    <cfRule type="expression" dxfId="389" priority="316" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="466" priority="317" stopIfTrue="1">
+    <cfRule type="expression" dxfId="388" priority="317" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="465" priority="318" stopIfTrue="1">
+    <cfRule type="expression" dxfId="387" priority="318" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S61 Z61:IO61 T59:Y59">
-    <cfRule type="expression" dxfId="464" priority="322" stopIfTrue="1">
+    <cfRule type="expression" dxfId="386" priority="322" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="463" priority="323" stopIfTrue="1">
+    <cfRule type="expression" dxfId="385" priority="323" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="462" priority="324" stopIfTrue="1">
+    <cfRule type="expression" dxfId="384" priority="324" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S17:IO17">
-    <cfRule type="expression" dxfId="461" priority="646" stopIfTrue="1">
+    <cfRule type="expression" dxfId="383" priority="646" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="460" priority="647" stopIfTrue="1">
+    <cfRule type="expression" dxfId="382" priority="647" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="459" priority="648" stopIfTrue="1">
+    <cfRule type="expression" dxfId="381" priority="648" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB18:IO19">
-    <cfRule type="expression" dxfId="458" priority="679" stopIfTrue="1">
+    <cfRule type="expression" dxfId="380" priority="679" stopIfTrue="1">
       <formula>$E13="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="457" priority="680" stopIfTrue="1">
+    <cfRule type="expression" dxfId="379" priority="680" stopIfTrue="1">
       <formula>$E13="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="456" priority="681" stopIfTrue="1">
+    <cfRule type="expression" dxfId="378" priority="681" stopIfTrue="1">
       <formula>OR($E13="終了",$E13="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z27:IO27">
-    <cfRule type="expression" dxfId="455" priority="718" stopIfTrue="1">
+    <cfRule type="expression" dxfId="377" priority="718" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="454" priority="719" stopIfTrue="1">
+    <cfRule type="expression" dxfId="376" priority="719" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="453" priority="720" stopIfTrue="1">
+    <cfRule type="expression" dxfId="375" priority="720" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S41 Z41:IO41 S35:S39 Z35:IO39">
-    <cfRule type="expression" dxfId="452" priority="814" stopIfTrue="1">
+    <cfRule type="expression" dxfId="374" priority="814" stopIfTrue="1">
       <formula>$E17="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="451" priority="815" stopIfTrue="1">
+    <cfRule type="expression" dxfId="373" priority="815" stopIfTrue="1">
       <formula>$E17="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="450" priority="816" stopIfTrue="1">
+    <cfRule type="expression" dxfId="372" priority="816" stopIfTrue="1">
       <formula>OR($E17="終了",$E17="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S40 Z40:IO40">
-    <cfRule type="expression" dxfId="449" priority="871" stopIfTrue="1">
+    <cfRule type="expression" dxfId="371" priority="871" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="448" priority="872" stopIfTrue="1">
+    <cfRule type="expression" dxfId="370" priority="872" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="447" priority="873" stopIfTrue="1">
+    <cfRule type="expression" dxfId="369" priority="873" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP21:XFD22 IP24:XFD25 IP28:XFD29">
-    <cfRule type="expression" dxfId="446" priority="922" stopIfTrue="1">
+    <cfRule type="expression" dxfId="368" priority="922" stopIfTrue="1">
       <formula>$D17="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="445" priority="923" stopIfTrue="1">
+    <cfRule type="expression" dxfId="367" priority="923" stopIfTrue="1">
       <formula>$D17="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="444" priority="924" stopIfTrue="1">
+    <cfRule type="expression" dxfId="366" priority="924" stopIfTrue="1">
       <formula>OR($D17="終了",$D17="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP57:XFD57">
-    <cfRule type="expression" dxfId="443" priority="952" stopIfTrue="1">
+    <cfRule type="expression" dxfId="365" priority="952" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="442" priority="953" stopIfTrue="1">
+    <cfRule type="expression" dxfId="364" priority="953" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="441" priority="954" stopIfTrue="1">
+    <cfRule type="expression" dxfId="363" priority="954" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I203:M65439">
-    <cfRule type="expression" dxfId="440" priority="955" stopIfTrue="1">
+    <cfRule type="expression" dxfId="362" priority="955" stopIfTrue="1">
       <formula>$D203="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="439" priority="956" stopIfTrue="1">
+    <cfRule type="expression" dxfId="361" priority="956" stopIfTrue="1">
       <formula>$D203="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="438" priority="957" stopIfTrue="1">
+    <cfRule type="expression" dxfId="360" priority="957" stopIfTrue="1">
       <formula>OR($D203="終了",$D203="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD48:IO48 T48:U48">
-    <cfRule type="expression" dxfId="434" priority="1048" stopIfTrue="1">
+    <cfRule type="expression" dxfId="359" priority="1048" stopIfTrue="1">
       <formula>$E24="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="433" priority="1049" stopIfTrue="1">
+    <cfRule type="expression" dxfId="358" priority="1049" stopIfTrue="1">
       <formula>$E24="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="432" priority="1050" stopIfTrue="1">
+    <cfRule type="expression" dxfId="357" priority="1050" stopIfTrue="1">
       <formula>OR($E24="終了",$E24="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP36:XFD36">
-    <cfRule type="expression" dxfId="431" priority="1063" stopIfTrue="1">
+    <cfRule type="expression" dxfId="356" priority="1063" stopIfTrue="1">
       <formula>$D38="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="430" priority="1064" stopIfTrue="1">
+    <cfRule type="expression" dxfId="355" priority="1064" stopIfTrue="1">
       <formula>$D38="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="429" priority="1065" stopIfTrue="1">
+    <cfRule type="expression" dxfId="354" priority="1065" stopIfTrue="1">
       <formula>OR($D38="終了",$D38="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S25:IO25">
-    <cfRule type="expression" dxfId="428" priority="1177" stopIfTrue="1">
+    <cfRule type="expression" dxfId="353" priority="1177" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="427" priority="1178" stopIfTrue="1">
+    <cfRule type="expression" dxfId="352" priority="1178" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="426" priority="1179" stopIfTrue="1">
+    <cfRule type="expression" dxfId="351" priority="1179" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD50:IO50">
-    <cfRule type="expression" dxfId="425" priority="1180" stopIfTrue="1">
+    <cfRule type="expression" dxfId="350" priority="1180" stopIfTrue="1">
       <formula>$E24="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="424" priority="1181" stopIfTrue="1">
+    <cfRule type="expression" dxfId="349" priority="1181" stopIfTrue="1">
       <formula>$E24="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="423" priority="1182" stopIfTrue="1">
+    <cfRule type="expression" dxfId="348" priority="1182" stopIfTrue="1">
       <formula>OR($E24="終了",$E24="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP6:XFD10">
-    <cfRule type="expression" dxfId="422" priority="1204" stopIfTrue="1">
+    <cfRule type="expression" dxfId="347" priority="1204" stopIfTrue="1">
       <formula>$D8="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="421" priority="1205" stopIfTrue="1">
+    <cfRule type="expression" dxfId="346" priority="1205" stopIfTrue="1">
       <formula>$D8="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="420" priority="1206" stopIfTrue="1">
+    <cfRule type="expression" dxfId="345" priority="1206" stopIfTrue="1">
       <formula>OR($D8="終了",$D8="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP15:XFD17 IP11:XFD11">
-    <cfRule type="expression" dxfId="419" priority="1207" stopIfTrue="1">
+    <cfRule type="expression" dxfId="344" priority="1207" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="418" priority="1208" stopIfTrue="1">
+    <cfRule type="expression" dxfId="343" priority="1208" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="417" priority="1209" stopIfTrue="1">
+    <cfRule type="expression" dxfId="342" priority="1209" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP12:XFD14">
-    <cfRule type="expression" dxfId="416" priority="1984" stopIfTrue="1">
+    <cfRule type="expression" dxfId="341" priority="1984" stopIfTrue="1">
       <formula>$D13="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="415" priority="1985" stopIfTrue="1">
+    <cfRule type="expression" dxfId="340" priority="1985" stopIfTrue="1">
       <formula>$D13="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="414" priority="1986" stopIfTrue="1">
+    <cfRule type="expression" dxfId="339" priority="1986" stopIfTrue="1">
       <formula>OR($D13="終了",$D13="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S7:IO8 C7:R7 S11:IO11 I11 I15 I19 I23 I27 I31 I35 K28:R28 K35:R35">
-    <cfRule type="expression" dxfId="413" priority="1987" stopIfTrue="1">
+    <cfRule type="expression" dxfId="338" priority="1987" stopIfTrue="1">
       <formula>$E8="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="412" priority="1988" stopIfTrue="1">
+    <cfRule type="expression" dxfId="337" priority="1988" stopIfTrue="1">
       <formula>$E8="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="411" priority="1989" stopIfTrue="1">
+    <cfRule type="expression" dxfId="336" priority="1989" stopIfTrue="1">
       <formula>OR($E8="終了",$E8="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP23:XFD23 IP48:XFD56">
-    <cfRule type="expression" dxfId="410" priority="2011" stopIfTrue="1">
+    <cfRule type="expression" dxfId="335" priority="2011" stopIfTrue="1">
       <formula>$D18="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="409" priority="2012" stopIfTrue="1">
+    <cfRule type="expression" dxfId="334" priority="2012" stopIfTrue="1">
       <formula>$D18="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="408" priority="2013" stopIfTrue="1">
+    <cfRule type="expression" dxfId="333" priority="2013" stopIfTrue="1">
       <formula>OR($D18="終了",$D18="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD46:IO46">
-    <cfRule type="expression" dxfId="407" priority="2047" stopIfTrue="1">
+    <cfRule type="expression" dxfId="332" priority="2047" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="406" priority="2048" stopIfTrue="1">
+    <cfRule type="expression" dxfId="331" priority="2048" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="405" priority="2049" stopIfTrue="1">
+    <cfRule type="expression" dxfId="330" priority="2049" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP26:XFD26 IP35:XFD35">
-    <cfRule type="expression" dxfId="404" priority="2065" stopIfTrue="1">
+    <cfRule type="expression" dxfId="329" priority="2065" stopIfTrue="1">
       <formula>$D23="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="403" priority="2066" stopIfTrue="1">
+    <cfRule type="expression" dxfId="328" priority="2066" stopIfTrue="1">
       <formula>$D23="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="402" priority="2067" stopIfTrue="1">
+    <cfRule type="expression" dxfId="327" priority="2067" stopIfTrue="1">
       <formula>OR($D23="終了",$D23="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP27:XFD27">
-    <cfRule type="expression" dxfId="401" priority="2071" stopIfTrue="1">
+    <cfRule type="expression" dxfId="326" priority="2071" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="400" priority="2072" stopIfTrue="1">
+    <cfRule type="expression" dxfId="325" priority="2072" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="399" priority="2073" stopIfTrue="1">
+    <cfRule type="expression" dxfId="324" priority="2073" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="398" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="323" priority="52" stopIfTrue="1">
       <formula>$E7="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="397" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="322" priority="53" stopIfTrue="1">
       <formula>$E7="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="396" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="321" priority="54" stopIfTrue="1">
       <formula>OR($E7="終了",$E7="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP31:XFD31">
-    <cfRule type="expression" dxfId="395" priority="2170" stopIfTrue="1">
+    <cfRule type="expression" dxfId="320" priority="2170" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="394" priority="2171" stopIfTrue="1">
+    <cfRule type="expression" dxfId="319" priority="2171" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="393" priority="2172" stopIfTrue="1">
+    <cfRule type="expression" dxfId="318" priority="2172" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP38:XFD39">
-    <cfRule type="expression" dxfId="392" priority="2278" stopIfTrue="1">
+    <cfRule type="expression" dxfId="317" priority="2278" stopIfTrue="1">
       <formula>$D33="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="391" priority="2279" stopIfTrue="1">
+    <cfRule type="expression" dxfId="316" priority="2279" stopIfTrue="1">
       <formula>$D33="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="390" priority="2280" stopIfTrue="1">
+    <cfRule type="expression" dxfId="315" priority="2280" stopIfTrue="1">
       <formula>OR($D33="終了",$D33="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP42:XFD42">
-    <cfRule type="expression" dxfId="389" priority="2296" stopIfTrue="1">
+    <cfRule type="expression" dxfId="314" priority="2296" stopIfTrue="1">
       <formula>$D26="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="388" priority="2297" stopIfTrue="1">
+    <cfRule type="expression" dxfId="313" priority="2297" stopIfTrue="1">
       <formula>$D26="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="387" priority="2298" stopIfTrue="1">
+    <cfRule type="expression" dxfId="312" priority="2298" stopIfTrue="1">
       <formula>OR($D26="終了",$D26="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP41:XFD41">
-    <cfRule type="expression" dxfId="386" priority="2320" stopIfTrue="1">
+    <cfRule type="expression" dxfId="311" priority="2320" stopIfTrue="1">
       <formula>$D35="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="385" priority="2321" stopIfTrue="1">
+    <cfRule type="expression" dxfId="310" priority="2321" stopIfTrue="1">
       <formula>$D35="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="384" priority="2322" stopIfTrue="1">
+    <cfRule type="expression" dxfId="309" priority="2322" stopIfTrue="1">
       <formula>OR($D35="終了",$D35="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP32:XFD33">
-    <cfRule type="expression" dxfId="383" priority="3046" stopIfTrue="1">
+    <cfRule type="expression" dxfId="308" priority="3046" stopIfTrue="1">
       <formula>$D29="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="382" priority="3047" stopIfTrue="1">
+    <cfRule type="expression" dxfId="307" priority="3047" stopIfTrue="1">
       <formula>$D29="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="381" priority="3048" stopIfTrue="1">
+    <cfRule type="expression" dxfId="306" priority="3048" stopIfTrue="1">
       <formula>OR($D29="終了",$D29="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP30:XFD30">
-    <cfRule type="expression" dxfId="380" priority="3061" stopIfTrue="1">
+    <cfRule type="expression" dxfId="305" priority="3061" stopIfTrue="1">
       <formula>$D28="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="379" priority="3062" stopIfTrue="1">
+    <cfRule type="expression" dxfId="304" priority="3062" stopIfTrue="1">
       <formula>$D28="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="378" priority="3063" stopIfTrue="1">
+    <cfRule type="expression" dxfId="303" priority="3063" stopIfTrue="1">
       <formula>OR($D28="終了",$D28="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP40:XFD40">
-    <cfRule type="expression" dxfId="377" priority="3085" stopIfTrue="1">
+    <cfRule type="expression" dxfId="302" priority="3085" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="376" priority="3086" stopIfTrue="1">
+    <cfRule type="expression" dxfId="301" priority="3086" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="375" priority="3087" stopIfTrue="1">
+    <cfRule type="expression" dxfId="300" priority="3087" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62">
-    <cfRule type="expression" dxfId="374" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="299" priority="22" stopIfTrue="1">
       <formula>$E62="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="373" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="298" priority="23" stopIfTrue="1">
       <formula>$E62="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="372" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="297" priority="24" stopIfTrue="1">
       <formula>OR($E62="終了",$E62="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62:D62 F62">
-    <cfRule type="expression" dxfId="371" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="296" priority="25" stopIfTrue="1">
       <formula>$E62="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="370" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="295" priority="26" stopIfTrue="1">
       <formula>$E62="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="369" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="294" priority="27" stopIfTrue="1">
       <formula>OR($E62="終了",$E62="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP44:XFD44">
-    <cfRule type="expression" dxfId="365" priority="3739" stopIfTrue="1">
+    <cfRule type="expression" dxfId="293" priority="3739" stopIfTrue="1">
       <formula>$D39="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="364" priority="3740" stopIfTrue="1">
+    <cfRule type="expression" dxfId="292" priority="3740" stopIfTrue="1">
       <formula>$D39="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="363" priority="3741" stopIfTrue="1">
+    <cfRule type="expression" dxfId="291" priority="3741" stopIfTrue="1">
       <formula>OR($D39="終了",$D39="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP43:XFD43">
-    <cfRule type="expression" dxfId="362" priority="3760" stopIfTrue="1">
+    <cfRule type="expression" dxfId="290" priority="3760" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="361" priority="3761" stopIfTrue="1">
+    <cfRule type="expression" dxfId="289" priority="3761" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="360" priority="3762" stopIfTrue="1">
+    <cfRule type="expression" dxfId="288" priority="3762" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP45:XFD47">
-    <cfRule type="expression" dxfId="359" priority="3823" stopIfTrue="1">
+    <cfRule type="expression" dxfId="287" priority="3823" stopIfTrue="1">
       <formula>$D41="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="358" priority="3824" stopIfTrue="1">
+    <cfRule type="expression" dxfId="286" priority="3824" stopIfTrue="1">
       <formula>$D41="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="357" priority="3825" stopIfTrue="1">
+    <cfRule type="expression" dxfId="285" priority="3825" stopIfTrue="1">
       <formula>OR($D41="終了",$D41="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37">
-    <cfRule type="expression" dxfId="356" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="284" priority="13" stopIfTrue="1">
       <formula>$E37="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="355" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="283" priority="14" stopIfTrue="1">
       <formula>$E37="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="354" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="282" priority="15" stopIfTrue="1">
       <formula>OR($E37="終了",$E37="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP34:XFD34">
-    <cfRule type="expression" dxfId="353" priority="3922" stopIfTrue="1">
+    <cfRule type="expression" dxfId="281" priority="3922" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="352" priority="3923" stopIfTrue="1">
+    <cfRule type="expression" dxfId="280" priority="3923" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="351" priority="3924" stopIfTrue="1">
+    <cfRule type="expression" dxfId="279" priority="3924" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP37:XFD37">
-    <cfRule type="expression" dxfId="350" priority="3961" stopIfTrue="1">
+    <cfRule type="expression" dxfId="278" priority="3961" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="349" priority="3962" stopIfTrue="1">
+    <cfRule type="expression" dxfId="277" priority="3962" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="348" priority="3963" stopIfTrue="1">
+    <cfRule type="expression" dxfId="276" priority="3963" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S34 Z34:IO34 T32:Y32">
-    <cfRule type="expression" dxfId="347" priority="1150" stopIfTrue="1">
+    <cfRule type="expression" dxfId="275" priority="1150" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="346" priority="1151" stopIfTrue="1">
+    <cfRule type="expression" dxfId="274" priority="1151" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="345" priority="1152" stopIfTrue="1">
+    <cfRule type="expression" dxfId="273" priority="1152" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IP18:XFD20">
-    <cfRule type="expression" dxfId="344" priority="1156" stopIfTrue="1">
+    <cfRule type="expression" dxfId="272" priority="1156" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="343" priority="1157" stopIfTrue="1">
+    <cfRule type="expression" dxfId="271" priority="1157" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="342" priority="1158" stopIfTrue="1">
+    <cfRule type="expression" dxfId="270" priority="1158" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C122">
-    <cfRule type="expression" dxfId="341" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="269" priority="10" stopIfTrue="1">
       <formula>$E122="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="340" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="268" priority="11" stopIfTrue="1">
       <formula>$E122="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="339" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="267" priority="12" stopIfTrue="1">
       <formula>OR($E122="終了",$E122="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C124">
-    <cfRule type="expression" dxfId="338" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="266" priority="7" stopIfTrue="1">
       <formula>$E123="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="337" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="265" priority="8" stopIfTrue="1">
       <formula>$E123="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="336" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="264" priority="9" stopIfTrue="1">
       <formula>OR($E123="終了",$E123="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C125">
-    <cfRule type="expression" dxfId="335" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="263" priority="4" stopIfTrue="1">
       <formula>$E124="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="334" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="262" priority="5" stopIfTrue="1">
       <formula>$E124="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="333" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="261" priority="6" stopIfTrue="1">
       <formula>OR($E124="終了",$E124="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C126">
-    <cfRule type="expression" dxfId="332" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="260" priority="1" stopIfTrue="1">
       <formula>$E125="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="331" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="259" priority="2" stopIfTrue="1">
       <formula>$E125="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="330" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="258" priority="3" stopIfTrue="1">
       <formula>OR($E125="終了",$E125="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T45:U45 T51:Y51">
-    <cfRule type="expression" dxfId="329" priority="3994" stopIfTrue="1">
+    <cfRule type="expression" dxfId="257" priority="3994" stopIfTrue="1">
       <formula>$E24="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="328" priority="3995" stopIfTrue="1">
+    <cfRule type="expression" dxfId="256" priority="3995" stopIfTrue="1">
       <formula>$E24="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="327" priority="3996" stopIfTrue="1">
+    <cfRule type="expression" dxfId="255" priority="3996" stopIfTrue="1">
       <formula>OR($E24="終了",$E24="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T46:U46">
-    <cfRule type="expression" dxfId="326" priority="4021" stopIfTrue="1">
+    <cfRule type="expression" dxfId="254" priority="4021" stopIfTrue="1">
       <formula>$E24="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="325" priority="4022" stopIfTrue="1">
+    <cfRule type="expression" dxfId="253" priority="4022" stopIfTrue="1">
       <formula>$E24="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="324" priority="4023" stopIfTrue="1">
+    <cfRule type="expression" dxfId="252" priority="4023" stopIfTrue="1">
       <formula>OR($E24="終了",$E24="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T33:Y35">
-    <cfRule type="expression" dxfId="323" priority="4030" stopIfTrue="1">
+    <cfRule type="expression" dxfId="251" priority="4030" stopIfTrue="1">
       <formula>$E17="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="322" priority="4031" stopIfTrue="1">
+    <cfRule type="expression" dxfId="250" priority="4031" stopIfTrue="1">
       <formula>$E17="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="321" priority="4032" stopIfTrue="1">
+    <cfRule type="expression" dxfId="249" priority="4032" stopIfTrue="1">
       <formula>OR($E17="終了",$E17="完了")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32802,45 +32231,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="8" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="100" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="99" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="105" t="s">
+      <c r="C1" s="100" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="106" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="99" t="s">
+      <c r="E1" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="102" t="s">
+      <c r="F1" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="H1" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="I1" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="99" t="s">
+      <c r="J1" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="110" t="s">
+      <c r="K1" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="110"/>
-      <c r="M1" s="110"/>
-      <c r="N1" s="110"/>
-      <c r="O1" s="110"/>
-      <c r="P1" s="110"/>
-      <c r="Q1" s="110"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
       <c r="R1" s="71"/>
       <c r="S1" s="71"/>
       <c r="T1" s="71"/>
@@ -32848,16 +32277,16 @@
       <c r="V1" s="71"/>
     </row>
     <row r="2" spans="1:22" s="8" customFormat="1">
-      <c r="A2" s="99"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="99"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="100"/>
       <c r="K2" s="23" t="s">
         <v>140</v>
       </c>
@@ -32881,31 +32310,31 @@
       </c>
     </row>
     <row r="3" spans="1:22" s="8" customFormat="1">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="99"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="100"/>
       <c r="K3" s="20">
         <f>INT(($K$4-(COLUMN()-COLUMN($K4))*($K$4/COUNTA($K$2:$Q$2))))</f>
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L3" s="20">
         <f t="shared" ref="L3:Q3" si="0">INT(($K$4-(COLUMN()-COLUMN($K4))*($K$4/COUNTA($K$2:$Q$2))))</f>
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M3" s="20">
         <f t="shared" si="0"/>
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N3" s="20">
         <f t="shared" si="0"/>
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O3" s="20">
         <f t="shared" si="0"/>
@@ -32913,7 +32342,7 @@
       </c>
       <c r="P3" s="20">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q3" s="20">
         <f t="shared" si="0"/>
@@ -32921,19 +32350,19 @@
       </c>
     </row>
     <row r="4" spans="1:22" s="8" customFormat="1">
-      <c r="A4" s="99"/>
-      <c r="B4" s="100"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="99"/>
+      <c r="A4" s="100"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="100"/>
       <c r="K4" s="21">
         <f>SUM(K5:K200)</f>
-        <v>235</v>
+        <v>233.5</v>
       </c>
       <c r="L4" s="21">
         <f t="shared" ref="L4:Q4" si="1">SUM(L5:L45)</f>
@@ -33259,7 +32688,7 @@
       <c r="A14" s="16">
         <v>10</v>
       </c>
-      <c r="B14" s="111"/>
+      <c r="B14" s="97"/>
       <c r="C14" s="83"/>
       <c r="D14" s="83"/>
       <c r="E14" s="84"/>
@@ -34292,7 +33721,7 @@
         <v>66</v>
       </c>
       <c r="V39" s="10">
-        <f t="shared" ref="V38:V43" ca="1" si="9">T39-U39</f>
+        <f t="shared" ref="V39:V43" ca="1" si="9">T39-U39</f>
         <v>2</v>
       </c>
       <c r="W39" s="14">
@@ -34459,18 +33888,18 @@
       </c>
       <c r="U42" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>20.5</v>
+        <v>19</v>
       </c>
       <c r="V42" s="10">
         <f t="shared" ca="1" si="9"/>
-        <v>11.5</v>
+        <v>13</v>
       </c>
       <c r="W42" s="14">
         <v>0</v>
       </c>
       <c r="X42" s="15">
         <f t="shared" ca="1" si="10"/>
-        <v>20.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:24">
@@ -36463,7 +35892,7 @@
       <c r="C96" s="18"/>
       <c r="D96" s="18"/>
       <c r="E96" s="12" t="str">
-        <f t="shared" ref="E79:E142" si="14">IF(ISBLANK($B96),"",IF(ISBLANK($G96),"未着手",IF($J96=0,"完了","作業中")))</f>
+        <f t="shared" ref="E96:E142" si="14">IF(ISBLANK($B96),"",IF(ISBLANK($G96),"未着手",IF($J96=0,"完了","作業中")))</f>
         <v/>
       </c>
       <c r="F96" s="4"/>
@@ -36471,7 +35900,7 @@
       <c r="H96" s="19"/>
       <c r="I96" s="19"/>
       <c r="J96" s="12" t="str">
-        <f t="shared" ref="J48:J111" ca="1" si="15">IF(ISBLANK(K96)=FALSE,OFFSET(J96,0,COUNTA(K96:Q96)),"")</f>
+        <f t="shared" ref="J96:J111" ca="1" si="15">IF(ISBLANK(K96)=FALSE,OFFSET(J96,0,COUNTA(K96:Q96)),"")</f>
         <v/>
       </c>
       <c r="K96" s="22"/>
@@ -36523,7 +35952,7 @@
       </c>
       <c r="E98" s="12" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>作業中</v>
+        <v>完了</v>
       </c>
       <c r="F98" s="4">
         <v>43104</v>
@@ -36535,14 +35964,14 @@
         <v>3</v>
       </c>
       <c r="I98" s="19">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="J98" s="12">
         <f t="shared" ca="1" si="15"/>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K98" s="22">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="L98" s="22"/>
       <c r="M98" s="22"/>
@@ -37037,7 +36466,7 @@
       <c r="H112" s="19"/>
       <c r="I112" s="19"/>
       <c r="J112" s="12" t="str">
-        <f t="shared" ref="J112:J118" ca="1" si="17">IF(ISBLANK(K112)=FALSE,OFFSET(J112,0,COUNTA(K112:Q112)),"")</f>
+        <f t="shared" ref="J112" ca="1" si="17">IF(ISBLANK(K112)=FALSE,OFFSET(J112,0,COUNTA(K112:Q112)),"")</f>
         <v/>
       </c>
       <c r="K112" s="22"/>
@@ -37063,7 +36492,7 @@
       <c r="H113" s="77"/>
       <c r="I113" s="77"/>
       <c r="J113" s="75" t="str">
-        <f t="shared" ref="J113:J125" ca="1" si="18">IF(ISBLANK(K113)=FALSE,OFFSET(J113,0,COUNTA(K113:R113)),"")</f>
+        <f t="shared" ref="J113:J120" ca="1" si="18">IF(ISBLANK(K113)=FALSE,OFFSET(J113,0,COUNTA(K113:R113)),"")</f>
         <v/>
       </c>
       <c r="K113" s="78"/>
@@ -37349,7 +36778,7 @@
       <c r="H121" s="19"/>
       <c r="I121" s="19"/>
       <c r="J121" s="12" t="str">
-        <f t="shared" ref="J119:J182" ca="1" si="20">IF(ISBLANK(K121)=FALSE,OFFSET(J121,0,COUNTA(K121:Q121)),"")</f>
+        <f t="shared" ref="J121:J182" ca="1" si="20">IF(ISBLANK(K121)=FALSE,OFFSET(J121,0,COUNTA(K121:Q121)),"")</f>
         <v/>
       </c>
       <c r="K121" s="22"/>
@@ -39682,827 +39111,827 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <conditionalFormatting sqref="D205:D65389">
-    <cfRule type="expression" dxfId="308" priority="196" stopIfTrue="1">
+    <cfRule type="expression" dxfId="236" priority="196" stopIfTrue="1">
       <formula>D205="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="307" priority="197" stopIfTrue="1">
+    <cfRule type="expression" dxfId="235" priority="197" stopIfTrue="1">
       <formula>D205="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="306" priority="198" stopIfTrue="1">
+    <cfRule type="expression" dxfId="234" priority="198" stopIfTrue="1">
       <formula>OR(D205="終了",D205="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO5:XFD5">
-    <cfRule type="expression" dxfId="305" priority="199" stopIfTrue="1">
+    <cfRule type="expression" dxfId="233" priority="199" stopIfTrue="1">
       <formula>$D5="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="304" priority="200" stopIfTrue="1">
+    <cfRule type="expression" dxfId="232" priority="200" stopIfTrue="1">
       <formula>$D5="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="303" priority="201" stopIfTrue="1">
+    <cfRule type="expression" dxfId="231" priority="201" stopIfTrue="1">
       <formula>OR($D5="終了",$D5="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B205:B65389">
-    <cfRule type="expression" dxfId="302" priority="202" stopIfTrue="1">
+    <cfRule type="expression" dxfId="230" priority="202" stopIfTrue="1">
       <formula>D205="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="301" priority="203" stopIfTrue="1">
+    <cfRule type="expression" dxfId="229" priority="203" stopIfTrue="1">
       <formula>D205="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="300" priority="204" stopIfTrue="1">
+    <cfRule type="expression" dxfId="228" priority="204" stopIfTrue="1">
       <formula>OR(D205="終了",D205="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C205:C65389">
-    <cfRule type="expression" dxfId="299" priority="205" stopIfTrue="1">
+    <cfRule type="expression" dxfId="227" priority="205" stopIfTrue="1">
       <formula>D205="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="298" priority="206" stopIfTrue="1">
+    <cfRule type="expression" dxfId="226" priority="206" stopIfTrue="1">
       <formula>D205="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="297" priority="207" stopIfTrue="1">
+    <cfRule type="expression" dxfId="225" priority="207" stopIfTrue="1">
       <formula>OR(D205="終了",D205="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E205:J65389">
-    <cfRule type="expression" dxfId="296" priority="208" stopIfTrue="1">
+    <cfRule type="expression" dxfId="224" priority="208" stopIfTrue="1">
       <formula>$D205="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="295" priority="209" stopIfTrue="1">
+    <cfRule type="expression" dxfId="223" priority="209" stopIfTrue="1">
       <formula>$D205="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="294" priority="210" stopIfTrue="1">
+    <cfRule type="expression" dxfId="222" priority="210" stopIfTrue="1">
       <formula>OR($D205="終了",$D205="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:Q6 B7:Q7 D9 D11 C10 B11 E10:I10 A14:I15 A7:A12 A5:IN5 J8:J15 A96:J96 A16:A95 A100:J100 I98:J99 A97:A99 C97:J97 A101:A111 I101:J111 A112:J112 A126:J204 A113:A125 I121:J125 I17:J95 K8:Q204">
-    <cfRule type="expression" dxfId="2" priority="127" stopIfTrue="1">
+    <cfRule type="expression" dxfId="221" priority="127" stopIfTrue="1">
       <formula>$E5="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="128" stopIfTrue="1">
+    <cfRule type="expression" dxfId="220" priority="128" stopIfTrue="1">
       <formula>$E5="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="129" stopIfTrue="1">
+    <cfRule type="expression" dxfId="219" priority="129" stopIfTrue="1">
       <formula>OR($E5="終了",$E5="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6:IN6">
-    <cfRule type="expression" dxfId="293" priority="133" stopIfTrue="1">
+    <cfRule type="expression" dxfId="218" priority="133" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="292" priority="134" stopIfTrue="1">
+    <cfRule type="expression" dxfId="217" priority="134" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="291" priority="135" stopIfTrue="1">
+    <cfRule type="expression" dxfId="216" priority="135" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R9:IN10">
-    <cfRule type="expression" dxfId="290" priority="136" stopIfTrue="1">
+    <cfRule type="expression" dxfId="215" priority="136" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="289" priority="137" stopIfTrue="1">
+    <cfRule type="expression" dxfId="214" priority="137" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="288" priority="138" stopIfTrue="1">
+    <cfRule type="expression" dxfId="213" priority="138" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R12:IN12 R14:IN15 S13:IN13">
-    <cfRule type="expression" dxfId="287" priority="139" stopIfTrue="1">
+    <cfRule type="expression" dxfId="212" priority="139" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="286" priority="140" stopIfTrue="1">
+    <cfRule type="expression" dxfId="211" priority="140" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="285" priority="141" stopIfTrue="1">
+    <cfRule type="expression" dxfId="210" priority="141" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA19:IN19">
-    <cfRule type="expression" dxfId="284" priority="142" stopIfTrue="1">
+    <cfRule type="expression" dxfId="209" priority="142" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="283" priority="143" stopIfTrue="1">
+    <cfRule type="expression" dxfId="208" priority="143" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="282" priority="144" stopIfTrue="1">
+    <cfRule type="expression" dxfId="207" priority="144" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22:IN23 AA21:IN21">
-    <cfRule type="expression" dxfId="281" priority="145" stopIfTrue="1">
+    <cfRule type="expression" dxfId="206" priority="145" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="280" priority="146" stopIfTrue="1">
+    <cfRule type="expression" dxfId="205" priority="146" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="279" priority="147" stopIfTrue="1">
+    <cfRule type="expression" dxfId="204" priority="147" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R24:IN24">
-    <cfRule type="expression" dxfId="278" priority="151" stopIfTrue="1">
+    <cfRule type="expression" dxfId="203" priority="151" stopIfTrue="1">
       <formula>$E7="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="277" priority="152" stopIfTrue="1">
+    <cfRule type="expression" dxfId="202" priority="152" stopIfTrue="1">
       <formula>$E7="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="276" priority="153" stopIfTrue="1">
+    <cfRule type="expression" dxfId="201" priority="153" stopIfTrue="1">
       <formula>OR($E7="終了",$E7="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R25:IN25">
-    <cfRule type="expression" dxfId="275" priority="154" stopIfTrue="1">
+    <cfRule type="expression" dxfId="200" priority="154" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="274" priority="155" stopIfTrue="1">
+    <cfRule type="expression" dxfId="199" priority="155" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="273" priority="156" stopIfTrue="1">
+    <cfRule type="expression" dxfId="198" priority="156" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R43 AC43:IN44 S44:T44">
-    <cfRule type="expression" dxfId="272" priority="157" stopIfTrue="1">
+    <cfRule type="expression" dxfId="197" priority="157" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="271" priority="158" stopIfTrue="1">
+    <cfRule type="expression" dxfId="196" priority="158" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="270" priority="159" stopIfTrue="1">
+    <cfRule type="expression" dxfId="195" priority="159" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R29:R30 Y27:IN30">
-    <cfRule type="expression" dxfId="269" priority="160" stopIfTrue="1">
+    <cfRule type="expression" dxfId="194" priority="160" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="268" priority="161" stopIfTrue="1">
+    <cfRule type="expression" dxfId="193" priority="161" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="267" priority="162" stopIfTrue="1">
+    <cfRule type="expression" dxfId="192" priority="162" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U32:IN33">
-    <cfRule type="expression" dxfId="266" priority="163" stopIfTrue="1">
+    <cfRule type="expression" dxfId="191" priority="163" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="265" priority="164" stopIfTrue="1">
+    <cfRule type="expression" dxfId="190" priority="164" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="264" priority="165" stopIfTrue="1">
+    <cfRule type="expression" dxfId="189" priority="165" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U31:IN31">
-    <cfRule type="expression" dxfId="263" priority="166" stopIfTrue="1">
+    <cfRule type="expression" dxfId="188" priority="166" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="262" priority="167" stopIfTrue="1">
+    <cfRule type="expression" dxfId="187" priority="167" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="261" priority="168" stopIfTrue="1">
+    <cfRule type="expression" dxfId="186" priority="168" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R41:R42 Y41:IN42">
-    <cfRule type="expression" dxfId="260" priority="169" stopIfTrue="1">
+    <cfRule type="expression" dxfId="185" priority="169" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="259" priority="170" stopIfTrue="1">
+    <cfRule type="expression" dxfId="184" priority="170" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="258" priority="171" stopIfTrue="1">
+    <cfRule type="expression" dxfId="183" priority="171" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC48:IN48 S48:T48">
-    <cfRule type="expression" dxfId="257" priority="172" stopIfTrue="1">
+    <cfRule type="expression" dxfId="182" priority="172" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="256" priority="173" stopIfTrue="1">
+    <cfRule type="expression" dxfId="181" priority="173" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="255" priority="174" stopIfTrue="1">
+    <cfRule type="expression" dxfId="180" priority="174" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC50:IN50 S50:T50">
-    <cfRule type="expression" dxfId="254" priority="178" stopIfTrue="1">
+    <cfRule type="expression" dxfId="179" priority="178" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="253" priority="179" stopIfTrue="1">
+    <cfRule type="expression" dxfId="178" priority="179" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="252" priority="180" stopIfTrue="1">
+    <cfRule type="expression" dxfId="177" priority="180" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R56:IN56">
-    <cfRule type="expression" dxfId="251" priority="184" stopIfTrue="1">
+    <cfRule type="expression" dxfId="176" priority="184" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="250" priority="185" stopIfTrue="1">
+    <cfRule type="expression" dxfId="175" priority="185" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="249" priority="186" stopIfTrue="1">
+    <cfRule type="expression" dxfId="174" priority="186" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R53:IN55">
-    <cfRule type="expression" dxfId="248" priority="187" stopIfTrue="1">
+    <cfRule type="expression" dxfId="173" priority="187" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="247" priority="188" stopIfTrue="1">
+    <cfRule type="expression" dxfId="172" priority="188" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="246" priority="189" stopIfTrue="1">
+    <cfRule type="expression" dxfId="171" priority="189" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R57:IN58">
-    <cfRule type="expression" dxfId="245" priority="190" stopIfTrue="1">
+    <cfRule type="expression" dxfId="170" priority="190" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="244" priority="191" stopIfTrue="1">
+    <cfRule type="expression" dxfId="169" priority="191" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="243" priority="192" stopIfTrue="1">
+    <cfRule type="expression" dxfId="168" priority="192" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R59:IN59">
-    <cfRule type="expression" dxfId="242" priority="193" stopIfTrue="1">
+    <cfRule type="expression" dxfId="167" priority="193" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="241" priority="194" stopIfTrue="1">
+    <cfRule type="expression" dxfId="166" priority="194" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="240" priority="195" stopIfTrue="1">
+    <cfRule type="expression" dxfId="165" priority="195" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R16:IN16">
-    <cfRule type="expression" dxfId="239" priority="211" stopIfTrue="1">
+    <cfRule type="expression" dxfId="164" priority="211" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="238" priority="212" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="212" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="237" priority="213" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="213" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y26:IN26">
-    <cfRule type="expression" dxfId="236" priority="217" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="217" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="235" priority="218" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="218" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="234" priority="219" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="219" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R39 Y39:IN39">
-    <cfRule type="expression" dxfId="233" priority="226" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="226" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="232" priority="227" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="227" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="231" priority="228" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="228" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO56:XFD56">
-    <cfRule type="expression" dxfId="230" priority="235" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="235" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="229" priority="236" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="236" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="228" priority="237" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="237" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO43:XFD43">
-    <cfRule type="expression" dxfId="227" priority="253" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="253" stopIfTrue="1">
       <formula>$D14="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="226" priority="254" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="254" stopIfTrue="1">
       <formula>$D14="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="225" priority="255" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="255" stopIfTrue="1">
       <formula>OR($D14="終了",$D14="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9 B8:E8 E11:E12 B9:C9 E9 D10 D12 B10 C11:C12 B12 H12">
-    <cfRule type="expression" dxfId="224" priority="100" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="100" stopIfTrue="1">
       <formula>$E8="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="223" priority="101" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="101" stopIfTrue="1">
       <formula>$E8="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="222" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="102" stopIfTrue="1">
       <formula>OR($E8="終了",$E8="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8 H11">
-    <cfRule type="expression" dxfId="221" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="97" stopIfTrue="1">
       <formula>$E8="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="220" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="98" stopIfTrue="1">
       <formula>$E8="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="219" priority="99" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="99" stopIfTrue="1">
       <formula>OR($E8="終了",$E8="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:G9 F12:G12">
-    <cfRule type="expression" dxfId="218" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="94" stopIfTrue="1">
       <formula>$E9="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="217" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="95" stopIfTrue="1">
       <formula>$E9="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="216" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="96" stopIfTrue="1">
       <formula>OR($E9="終了",$E9="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:G8 F11:G11">
-    <cfRule type="expression" dxfId="215" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="91" stopIfTrue="1">
       <formula>$E8="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="214" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="92" stopIfTrue="1">
       <formula>$E8="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="213" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="93" stopIfTrue="1">
       <formula>OR($E8="終了",$E8="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R11:IN11 R7:IN8">
-    <cfRule type="expression" dxfId="212" priority="1252" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="1252" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="211" priority="1253" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="1253" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="210" priority="1254" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="1254" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA20:IN20">
-    <cfRule type="expression" dxfId="209" priority="1267" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="1267" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="208" priority="1268" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="1268" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="207" priority="1269" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="1269" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA17:IN18">
-    <cfRule type="expression" dxfId="206" priority="1282" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="1282" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="205" priority="1283" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="1283" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="204" priority="1284" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="1284" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO6:XFD14">
-    <cfRule type="expression" dxfId="203" priority="1297" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="1297" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="202" priority="1298" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="1298" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="1299" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="1299" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO15:XFD15">
-    <cfRule type="expression" dxfId="200" priority="1327" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="1327" stopIfTrue="1">
       <formula>$D7="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="199" priority="1328" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="1328" stopIfTrue="1">
       <formula>$D7="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="1329" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="1329" stopIfTrue="1">
       <formula>OR($D7="終了",$D7="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO16:XFD16">
-    <cfRule type="expression" dxfId="197" priority="1330" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="1330" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="1331" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="1331" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="1332" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="1332" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R52:IN52 AC45:IN46 S45:T46">
-    <cfRule type="expression" dxfId="194" priority="1342" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="1342" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="193" priority="1343" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="1343" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="1344" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="1344" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA51:IN51 S51:T51">
-    <cfRule type="expression" dxfId="191" priority="1351" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="1351" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="190" priority="1352" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="1352" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="1353" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="1353" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R40 Y40:IN40 R35:IN36">
-    <cfRule type="expression" dxfId="188" priority="1357" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="1357" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="1358" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="1358" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="1359" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="1359" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R37:R38 Y37:IN38">
-    <cfRule type="expression" dxfId="185" priority="1366" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="1366" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="1367" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="1367" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="183" priority="1368" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="1368" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO20:XFD42">
-    <cfRule type="expression" dxfId="182" priority="1372" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="1372" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="1373" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="1373" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="1374" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="1374" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC47:IN47 S47:T47">
-    <cfRule type="expression" dxfId="179" priority="1375" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="1375" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="1376" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="1376" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="177" priority="1377" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="1377" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S49:T49 AC49:IN49">
-    <cfRule type="expression" dxfId="176" priority="1384" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="1384" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="175" priority="1385" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="1385" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="1386" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="1386" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205:K65388">
-    <cfRule type="expression" dxfId="173" priority="1411" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="1411" stopIfTrue="1">
       <formula>$D206="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="1412" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="1412" stopIfTrue="1">
       <formula>$D206="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="1413" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="1413" stopIfTrue="1">
       <formula>OR($D206="終了",$D206="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L205:M65387">
-    <cfRule type="expression" dxfId="170" priority="1501" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="1501" stopIfTrue="1">
       <formula>$D207="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="1502" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="1502" stopIfTrue="1">
       <formula>$D207="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="1503" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="1503" stopIfTrue="1">
       <formula>OR($D207="終了",$D207="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO47:XFD55">
-    <cfRule type="expression" dxfId="167" priority="1789" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="1789" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="1790" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="1790" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="1791" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="1791" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO44:XFD46">
-    <cfRule type="expression" dxfId="164" priority="1798" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="1798" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="1799" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="1799" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="1800" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="1800" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:I13 A13:E13 R13">
-    <cfRule type="expression" dxfId="161" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="76" stopIfTrue="1">
       <formula>$E13="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="77" stopIfTrue="1">
       <formula>$E13="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="78" stopIfTrue="1">
       <formula>OR($E13="終了",$E13="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="158" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="73" stopIfTrue="1">
       <formula>$E13="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="74" stopIfTrue="1">
       <formula>$E13="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="75" stopIfTrue="1">
       <formula>OR($E13="終了",$E13="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I9 I11:I12">
-    <cfRule type="expression" dxfId="155" priority="256" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="256" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="257" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="257" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="258" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="258" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R34:IN34">
-    <cfRule type="expression" dxfId="152" priority="259" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="259" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="260" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="260" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="261" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="261" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IO17:XFD19">
-    <cfRule type="expression" dxfId="149" priority="262" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="262" stopIfTrue="1">
       <formula>#REF!="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="263" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="263" stopIfTrue="1">
       <formula>#REF!="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="264" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="264" stopIfTrue="1">
       <formula>OR(#REF!="終了",#REF!="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="expression" dxfId="143" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="67" stopIfTrue="1">
       <formula>$E16="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="68" stopIfTrue="1">
       <formula>$E16="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="69" stopIfTrue="1">
       <formula>OR($E16="終了",$E16="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:H25">
-    <cfRule type="expression" dxfId="116" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="61" stopIfTrue="1">
       <formula>$E18="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="62" stopIfTrue="1">
       <formula>$E18="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="63" stopIfTrue="1">
       <formula>OR($E18="終了",$E18="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:H17">
-    <cfRule type="expression" dxfId="113" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="64" stopIfTrue="1">
       <formula>$E18="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="65" stopIfTrue="1">
       <formula>$E18="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="66" stopIfTrue="1">
       <formula>OR($E18="終了",$E18="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="110" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="58" stopIfTrue="1">
       <formula>$E17="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="59" stopIfTrue="1">
       <formula>$E17="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="60" stopIfTrue="1">
       <formula>OR($E17="終了",$E17="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:H31">
-    <cfRule type="expression" dxfId="107" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="55" stopIfTrue="1">
       <formula>$E26="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="56" stopIfTrue="1">
       <formula>$E26="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="57" stopIfTrue="1">
       <formula>OR($E26="終了",$E26="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:H35">
-    <cfRule type="expression" dxfId="101" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="52" stopIfTrue="1">
       <formula>$E32="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="53" stopIfTrue="1">
       <formula>$E32="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="54" stopIfTrue="1">
       <formula>OR($E32="終了",$E32="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:H39">
-    <cfRule type="expression" dxfId="98" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="49" stopIfTrue="1">
       <formula>$E36="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="50" stopIfTrue="1">
       <formula>$E36="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="51" stopIfTrue="1">
       <formula>OR($E36="終了",$E36="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:E46 H46 B40:H45 B47:H47">
-    <cfRule type="expression" dxfId="95" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="46" stopIfTrue="1">
       <formula>$E40="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="47" stopIfTrue="1">
       <formula>$E40="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="48" stopIfTrue="1">
       <formula>OR($E40="終了",$E40="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46">
-    <cfRule type="expression" dxfId="92" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="40" stopIfTrue="1">
       <formula>$E46="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="41" stopIfTrue="1">
       <formula>$E46="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="42" stopIfTrue="1">
       <formula>OR($E46="終了",$E46="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:H50">
-    <cfRule type="expression" dxfId="86" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="37" stopIfTrue="1">
       <formula>$E50="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="38" stopIfTrue="1">
       <formula>$E50="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="39" stopIfTrue="1">
       <formula>OR($E50="終了",$E50="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:H49">
-    <cfRule type="expression" dxfId="77" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="34" stopIfTrue="1">
       <formula>$E48="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="35" stopIfTrue="1">
       <formula>$E48="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="36" stopIfTrue="1">
       <formula>OR($E48="終了",$E48="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91:B95 D91:D95 B51:D90 E51:H95">
-    <cfRule type="expression" dxfId="53" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="28" stopIfTrue="1">
       <formula>$E51="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="29" stopIfTrue="1">
       <formula>$E51="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="30" stopIfTrue="1">
       <formula>OR($E51="終了",$E51="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92">
-    <cfRule type="expression" dxfId="50" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="31" stopIfTrue="1">
       <formula>$E91="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="32" stopIfTrue="1">
       <formula>$E91="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="33" stopIfTrue="1">
       <formula>OR($E91="終了",$E91="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91">
-    <cfRule type="expression" dxfId="47" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="25" stopIfTrue="1">
       <formula>$E91="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="26" stopIfTrue="1">
       <formula>$E91="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="27" stopIfTrue="1">
       <formula>OR($E91="終了",$E91="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93">
-    <cfRule type="expression" dxfId="44" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="22" stopIfTrue="1">
       <formula>$E92="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="23" stopIfTrue="1">
       <formula>$E92="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="24" stopIfTrue="1">
       <formula>OR($E92="終了",$E92="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94">
-    <cfRule type="expression" dxfId="41" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="19" stopIfTrue="1">
       <formula>$E93="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="20" stopIfTrue="1">
       <formula>$E93="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="21" stopIfTrue="1">
       <formula>OR($E93="終了",$E93="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="expression" dxfId="38" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="16" stopIfTrue="1">
       <formula>$E94="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="17" stopIfTrue="1">
       <formula>$E94="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="18" stopIfTrue="1">
       <formula>OR($E94="終了",$E94="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98:H99">
-    <cfRule type="expression" dxfId="35" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="13" stopIfTrue="1">
       <formula>$E98="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="14" stopIfTrue="1">
       <formula>$E98="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="15" stopIfTrue="1">
       <formula>OR($E98="終了",$E98="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97">
-    <cfRule type="expression" dxfId="32" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="10" stopIfTrue="1">
       <formula>$E97="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="11" stopIfTrue="1">
       <formula>$E97="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="12" stopIfTrue="1">
       <formula>OR($E97="終了",$E97="完了")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101:H111">
-    <cfRule type="expression" dxfId="29" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="7" stopIfTrue="1">
       <formula>$E101="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="8" stopIfTrue="1">
       <formula>$E101="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="9" stopIfTrue="1">
       <formula>OR($E101="終了",$E101="完了")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40518,13 +39947,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:H125">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
       <formula>$E121="未着手"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
       <formula>$E121="作業中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
       <formula>OR($E121="終了",$E121="完了")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41413,13 +40842,13 @@
   <autoFilter ref="B1:K51"/>
   <phoneticPr fontId="4"/>
   <conditionalFormatting sqref="A2:K51">
-    <cfRule type="expression" dxfId="83" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
       <formula>$D2="要望"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>$D2="確認済"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>$D2="対応"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
A Text File For Gyan
</commit_message>
<xml_diff>
--- a/Godlibrary/BackLog.xlsx
+++ b/Godlibrary/BackLog.xlsx
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'スプリントバックログ(第3)'!$C$1:$D$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'スプリントバックログ(第4)'!$C$1:$D$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'スプリントバックログ(第5)'!$C$1:$C$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">デバッグシート!$B$1:$K$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">デバッグシート!$B$1:$K$52</definedName>
     <definedName name="重要度" localSheetId="1">OFFSET(#REF!,0,0,COUNTA(#REF!),1)</definedName>
     <definedName name="重要度" localSheetId="3">OFFSET(#REF!,0,0,COUNTA(#REF!),1)</definedName>
     <definedName name="重要度" localSheetId="4">OFFSET(#REF!,0,0,COUNTA(#REF!),1)</definedName>
@@ -802,7 +802,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="429">
   <si>
     <t>担当者</t>
   </si>
@@ -4236,19 +4236,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>ステージ2以降が直したヤツ反映されてない</t>
-    <rPh sb="5" eb="7">
-      <t>イコウ</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>ナオ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ハンエイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>アイテム管理からステータス翔べない</t>
     <rPh sb="4" eb="6">
       <t>カンリ</t>
@@ -4278,6 +4265,122 @@
     </rPh>
     <rPh sb="13" eb="14">
       <t>ワ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>編成画面統一</t>
+    <rPh sb="0" eb="4">
+      <t>ヘンセイガメン</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>トウイツ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>マップ上のステ画面でLVとかが反映されてない</t>
+    <rPh sb="3" eb="4">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ハンエイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>編成画面→マップを見るからだと9でステータス開けない</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンセイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>マップ上メニュー画面の整理</t>
+    <rPh sb="3" eb="4">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>セイリ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>マップ上メニューで設定からBGM音量いじろうとするとキャンセルができない？</t>
+    <rPh sb="3" eb="4">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>オンリョウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>編成画面　初回でのチラツキ</t>
+    <rPh sb="0" eb="4">
+      <t>ヘンセイガメン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ショカイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>マップ上のステ画面きれいにする</t>
+    <rPh sb="3" eb="4">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ガメン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>セーブデータ更新</t>
+    <rPh sb="6" eb="8">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>水沼</t>
+    <rPh sb="0" eb="2">
+      <t>ミズヌマ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>遠藤</t>
+    <rPh sb="0" eb="2">
+      <t>エンドウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>編成画面でカーソル動かない</t>
+    <rPh sb="0" eb="4">
+      <t>ヘンセイガメン</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ウゴ</t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
@@ -5031,6 +5134,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5038,12 +5147,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -15367,6 +15470,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -15480,6 +15584,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -15664,6 +15769,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -22215,7 +22321,7 @@
       <c r="C1" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="D1" s="105" t="s">
         <v>43</v>
       </c>
       <c r="E1" s="97" t="s">
@@ -22239,8 +22345,8 @@
       <c r="K1" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="106"/>
-      <c r="M1" s="107"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="104"/>
       <c r="N1" s="71"/>
       <c r="O1" s="71"/>
       <c r="P1" s="71"/>
@@ -22255,7 +22361,7 @@
       <c r="A2" s="97"/>
       <c r="B2" s="98"/>
       <c r="C2" s="98"/>
-      <c r="D2" s="104"/>
+      <c r="D2" s="106"/>
       <c r="E2" s="97"/>
       <c r="F2" s="100"/>
       <c r="G2" s="100"/>
@@ -22276,7 +22382,7 @@
       <c r="A3" s="97"/>
       <c r="B3" s="98"/>
       <c r="C3" s="98"/>
-      <c r="D3" s="104"/>
+      <c r="D3" s="106"/>
       <c r="E3" s="97"/>
       <c r="F3" s="100"/>
       <c r="G3" s="100"/>
@@ -22300,7 +22406,7 @@
       <c r="A4" s="97"/>
       <c r="B4" s="98"/>
       <c r="C4" s="99"/>
-      <c r="D4" s="105"/>
+      <c r="D4" s="107"/>
       <c r="E4" s="97"/>
       <c r="F4" s="100"/>
       <c r="G4" s="100"/>
@@ -24051,17 +24157,17 @@
   </sheetData>
   <autoFilter ref="C1:D123"/>
   <mergeCells count="11">
-    <mergeCell ref="G1:G4"/>
-    <mergeCell ref="H1:H4"/>
-    <mergeCell ref="I1:I4"/>
-    <mergeCell ref="J1:J4"/>
-    <mergeCell ref="K1:M1"/>
     <mergeCell ref="F1:F4"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
     <mergeCell ref="D1:D4"/>
     <mergeCell ref="E1:E4"/>
+    <mergeCell ref="G1:G4"/>
+    <mergeCell ref="H1:H4"/>
+    <mergeCell ref="I1:I4"/>
+    <mergeCell ref="J1:J4"/>
+    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <conditionalFormatting sqref="D43:D65414">
@@ -25211,7 +25317,7 @@
       <c r="C1" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="D1" s="105" t="s">
         <v>43</v>
       </c>
       <c r="E1" s="97" t="s">
@@ -25235,13 +25341,13 @@
       <c r="K1" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="106"/>
-      <c r="O1" s="106"/>
-      <c r="P1" s="106"/>
-      <c r="Q1" s="106"/>
-      <c r="R1" s="107"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="104"/>
       <c r="S1" s="71"/>
       <c r="T1" s="71"/>
       <c r="U1" s="71"/>
@@ -25252,7 +25358,7 @@
       <c r="A2" s="97"/>
       <c r="B2" s="98"/>
       <c r="C2" s="98"/>
-      <c r="D2" s="104"/>
+      <c r="D2" s="106"/>
       <c r="E2" s="97"/>
       <c r="F2" s="100"/>
       <c r="G2" s="100"/>
@@ -25288,7 +25394,7 @@
       <c r="A3" s="97"/>
       <c r="B3" s="98"/>
       <c r="C3" s="98"/>
-      <c r="D3" s="104"/>
+      <c r="D3" s="106"/>
       <c r="E3" s="97"/>
       <c r="F3" s="100"/>
       <c r="G3" s="100"/>
@@ -25332,7 +25438,7 @@
       <c r="A4" s="97"/>
       <c r="B4" s="98"/>
       <c r="C4" s="99"/>
-      <c r="D4" s="105"/>
+      <c r="D4" s="107"/>
       <c r="E4" s="97"/>
       <c r="F4" s="100"/>
       <c r="G4" s="100"/>
@@ -28820,7 +28926,7 @@
       <c r="C1" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="D1" s="105" t="s">
         <v>43</v>
       </c>
       <c r="E1" s="97" t="s">
@@ -28860,7 +28966,7 @@
       <c r="A2" s="97"/>
       <c r="B2" s="98"/>
       <c r="C2" s="98"/>
-      <c r="D2" s="104"/>
+      <c r="D2" s="106"/>
       <c r="E2" s="97"/>
       <c r="F2" s="100"/>
       <c r="G2" s="100"/>
@@ -28893,7 +28999,7 @@
       <c r="A3" s="97"/>
       <c r="B3" s="98"/>
       <c r="C3" s="98"/>
-      <c r="D3" s="104"/>
+      <c r="D3" s="106"/>
       <c r="E3" s="97"/>
       <c r="F3" s="100"/>
       <c r="G3" s="100"/>
@@ -28933,7 +29039,7 @@
       <c r="A4" s="97"/>
       <c r="B4" s="98"/>
       <c r="C4" s="99"/>
-      <c r="D4" s="105"/>
+      <c r="D4" s="107"/>
       <c r="E4" s="97"/>
       <c r="F4" s="100"/>
       <c r="G4" s="100"/>
@@ -28966,7 +29072,7 @@
       </c>
       <c r="Q4" s="21">
         <f t="shared" si="1"/>
-        <v>51.5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -30502,7 +30608,7 @@
       </c>
       <c r="E37" s="12" t="str">
         <f ca="1">IF(ISBLANK($B37),"",IF(ISBLANK($G37),"未着手",IF($J37=0,"完了","作業中")))</f>
-        <v>作業中</v>
+        <v>完了</v>
       </c>
       <c r="F37" s="4">
         <v>43096</v>
@@ -30518,7 +30624,7 @@
       </c>
       <c r="J37" s="12">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" s="22">
         <v>3</v>
@@ -30539,7 +30645,7 @@
         <v>2</v>
       </c>
       <c r="Q37" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S37" s="13"/>
       <c r="T37" s="13" t="s">
@@ -30650,7 +30756,7 @@
       </c>
       <c r="E39" s="12" t="str">
         <f ca="1">IF(ISBLANK($B39),"",IF(ISBLANK($G39),"未着手",IF($J39=0,"完了","作業中")))</f>
-        <v>作業中</v>
+        <v>完了</v>
       </c>
       <c r="F39" s="4">
         <v>43094</v>
@@ -30662,11 +30768,11 @@
         <v>6</v>
       </c>
       <c r="I39" s="19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J39" s="12">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39" s="22">
         <v>6</v>
@@ -30687,7 +30793,7 @@
         <v>3</v>
       </c>
       <c r="Q39" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S39" s="11" t="s">
         <v>92</v>
@@ -30698,18 +30804,18 @@
       </c>
       <c r="U39" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>34.5</v>
+        <v>31.5</v>
       </c>
       <c r="V39" s="10">
         <f t="shared" ref="V39:V43" ca="1" si="9">T39-U39</f>
-        <v>42.5</v>
+        <v>45.5</v>
       </c>
       <c r="W39" s="14">
         <v>0</v>
       </c>
       <c r="X39" s="15">
         <f t="shared" ref="X39:X43" ca="1" si="10">IF(W39&gt;U39,0,U39-W39)</f>
-        <v>34.5</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="40" spans="1:24">
@@ -30746,18 +30852,18 @@
       </c>
       <c r="U40" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="V40" s="10">
         <f t="shared" ca="1" si="9"/>
-        <v>20.5</v>
+        <v>21</v>
       </c>
       <c r="W40" s="14">
         <v>0</v>
       </c>
       <c r="X40" s="15">
         <f t="shared" ca="1" si="10"/>
-        <v>7.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:24">
@@ -34569,7 +34675,7 @@
       </c>
       <c r="E119" s="12" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>作業中</v>
+        <v>完了</v>
       </c>
       <c r="F119" s="4">
         <v>43119</v>
@@ -34581,11 +34687,11 @@
         <v>3</v>
       </c>
       <c r="I119" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J119" s="12">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K119" s="22">
         <v>3</v>
@@ -34606,7 +34712,7 @@
         <v>3</v>
       </c>
       <c r="Q119" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:17">
@@ -35202,7 +35308,7 @@
       <c r="D132" s="18"/>
       <c r="E132" s="12" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>作業中</v>
+        <v>完了</v>
       </c>
       <c r="F132" s="4">
         <v>43123</v>
@@ -35214,11 +35320,11 @@
         <v>1</v>
       </c>
       <c r="I132" s="19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J132" s="12">
         <f t="shared" ca="1" si="19"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K132" s="22">
         <v>1</v>
@@ -35239,7 +35345,7 @@
         <v>0.5</v>
       </c>
       <c r="Q132" s="22">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:17">
@@ -37126,17 +37232,17 @@
   </sheetData>
   <autoFilter ref="C1:D49"/>
   <mergeCells count="11">
+    <mergeCell ref="G1:G4"/>
+    <mergeCell ref="H1:H4"/>
+    <mergeCell ref="I1:I4"/>
+    <mergeCell ref="J1:J4"/>
+    <mergeCell ref="K1:Q1"/>
     <mergeCell ref="F1:F4"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
     <mergeCell ref="D1:D4"/>
     <mergeCell ref="E1:E4"/>
-    <mergeCell ref="G1:G4"/>
-    <mergeCell ref="H1:H4"/>
-    <mergeCell ref="I1:I4"/>
-    <mergeCell ref="J1:J4"/>
-    <mergeCell ref="K1:Q1"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <conditionalFormatting sqref="D192:D65359 C175:C191">
@@ -37999,7 +38105,7 @@
   <dimension ref="A1:W159"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -38160,7 +38266,7 @@
       </c>
       <c r="L4" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M4" s="21">
         <f t="shared" si="1"/>
@@ -39241,7 +39347,9 @@
       <c r="K37" s="22">
         <v>1</v>
       </c>
-      <c r="L37" s="22"/>
+      <c r="L37" s="22">
+        <v>1</v>
+      </c>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
       <c r="O37" s="22"/>
@@ -39347,7 +39455,9 @@
       <c r="K39" s="22">
         <v>0</v>
       </c>
-      <c r="L39" s="22"/>
+      <c r="L39" s="22">
+        <v>0</v>
+      </c>
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
       <c r="O39" s="22"/>
@@ -39411,7 +39521,9 @@
       <c r="K40" s="22">
         <v>0</v>
       </c>
-      <c r="L40" s="22"/>
+      <c r="L40" s="22">
+        <v>0</v>
+      </c>
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
       <c r="O40" s="22"/>
@@ -39475,7 +39587,9 @@
       <c r="K41" s="22">
         <v>0</v>
       </c>
-      <c r="L41" s="22"/>
+      <c r="L41" s="22">
+        <v>0</v>
+      </c>
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
       <c r="O41" s="22"/>
@@ -39537,7 +39651,9 @@
       <c r="K42" s="22">
         <v>3</v>
       </c>
-      <c r="L42" s="22"/>
+      <c r="L42" s="22">
+        <v>3</v>
+      </c>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
       <c r="O42" s="22"/>
@@ -39601,7 +39717,9 @@
       <c r="K43" s="22">
         <v>0</v>
       </c>
-      <c r="L43" s="22"/>
+      <c r="L43" s="22">
+        <v>0</v>
+      </c>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
       <c r="O43" s="22"/>
@@ -39665,7 +39783,9 @@
       <c r="K44" s="22">
         <v>0</v>
       </c>
-      <c r="L44" s="22"/>
+      <c r="L44" s="22">
+        <v>0</v>
+      </c>
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
       <c r="O44" s="22"/>
@@ -39887,23 +40007,41 @@
       <c r="A51" s="16">
         <v>47</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="18"/>
+      <c r="B51" s="17" t="s">
+        <v>418</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>427</v>
+      </c>
       <c r="D51" s="12" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
-      <c r="I51" s="12" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>完了</v>
+      </c>
+      <c r="E51" s="4">
+        <v>43144</v>
+      </c>
+      <c r="F51" s="4">
+        <v>43144</v>
+      </c>
+      <c r="G51" s="19">
+        <v>2</v>
+      </c>
+      <c r="H51" s="19">
+        <v>2</v>
+      </c>
+      <c r="I51" s="12">
         <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="J51" s="22"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="22"/>
+        <v>0</v>
+      </c>
+      <c r="J51" s="22">
+        <v>2</v>
+      </c>
+      <c r="K51" s="22">
+        <v>2</v>
+      </c>
+      <c r="L51" s="22">
+        <v>0</v>
+      </c>
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
       <c r="O51" s="22"/>
@@ -39913,23 +40051,41 @@
       <c r="A52" s="16">
         <v>48</v>
       </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="18"/>
+      <c r="B52" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>426</v>
+      </c>
       <c r="D52" s="12" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="12" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>作業中</v>
+      </c>
+      <c r="E52" s="4">
+        <v>43140</v>
+      </c>
+      <c r="F52" s="4">
+        <v>43140</v>
+      </c>
+      <c r="G52" s="19">
+        <v>4</v>
+      </c>
+      <c r="H52" s="19">
+        <v>2</v>
+      </c>
+      <c r="I52" s="12">
         <f t="shared" ref="I52:I115" ca="1" si="13">IF(ISBLANK(J52)=FALSE,OFFSET(I52,0,COUNTA(J52:P52)),"")</f>
-        <v/>
-      </c>
-      <c r="J52" s="22"/>
-      <c r="K52" s="22"/>
-      <c r="L52" s="22"/>
+        <v>2</v>
+      </c>
+      <c r="J52" s="22">
+        <v>4</v>
+      </c>
+      <c r="K52" s="22">
+        <v>4</v>
+      </c>
+      <c r="L52" s="22">
+        <v>2</v>
+      </c>
       <c r="M52" s="22"/>
       <c r="N52" s="22"/>
       <c r="O52" s="22"/>
@@ -42720,16 +42876,16 @@
   </sheetData>
   <autoFilter ref="C1:D16"/>
   <mergeCells count="10">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:E4"/>
     <mergeCell ref="F1:F4"/>
     <mergeCell ref="G1:G4"/>
     <mergeCell ref="H1:H4"/>
     <mergeCell ref="I1:I4"/>
     <mergeCell ref="J1:P1"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="E1:E4"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <conditionalFormatting sqref="D160:D65236">
@@ -42776,7 +42932,7 @@
       <formula>OR($D160="終了",$D160="完了")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:P24 J25:O26 P25:P29 J27:M29 J30:P159 B25:I159 A5:A159">
+  <conditionalFormatting sqref="B5:P24 J25:O26 P25:P29 J27:M29 B25:I159 A5:A159 J30:P159">
     <cfRule type="expression" dxfId="158" priority="82" stopIfTrue="1">
       <formula>$D5="未着手"</formula>
     </cfRule>
@@ -43303,11 +43459,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R51"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
   <cols>
@@ -43991,7 +44145,7 @@
       <c r="E33" s="32"/>
       <c r="F33" s="32"/>
       <c r="G33" s="92" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H33" s="32"/>
       <c r="I33" s="32"/>
@@ -44020,8 +44174,8 @@
       <c r="D35" s="32"/>
       <c r="E35" s="32"/>
       <c r="F35" s="32"/>
-      <c r="G35" s="92" t="s">
-        <v>416</v>
+      <c r="G35" s="89" t="s">
+        <v>417</v>
       </c>
       <c r="H35" s="32"/>
       <c r="I35" s="32"/>
@@ -44035,8 +44189,8 @@
       <c r="D36" s="32"/>
       <c r="E36" s="32"/>
       <c r="F36" s="32"/>
-      <c r="G36" s="89" t="s">
-        <v>418</v>
+      <c r="G36" s="92" t="s">
+        <v>424</v>
       </c>
       <c r="H36" s="32"/>
       <c r="I36" s="32"/>
@@ -44050,7 +44204,9 @@
       <c r="D37" s="32"/>
       <c r="E37" s="32"/>
       <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
+      <c r="G37" s="92" t="s">
+        <v>419</v>
+      </c>
       <c r="H37" s="32"/>
       <c r="I37" s="32"/>
       <c r="J37" s="32"/>
@@ -44063,7 +44219,9 @@
       <c r="D38" s="32"/>
       <c r="E38" s="32"/>
       <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
+      <c r="G38" s="89" t="s">
+        <v>420</v>
+      </c>
       <c r="H38" s="32"/>
       <c r="I38" s="32"/>
       <c r="J38" s="32"/>
@@ -44076,7 +44234,9 @@
       <c r="D39" s="32"/>
       <c r="E39" s="32"/>
       <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
+      <c r="G39" s="89" t="s">
+        <v>421</v>
+      </c>
       <c r="H39" s="32"/>
       <c r="I39" s="32"/>
       <c r="J39" s="32"/>
@@ -44089,7 +44249,9 @@
       <c r="D40" s="32"/>
       <c r="E40" s="32"/>
       <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
+      <c r="G40" s="89" t="s">
+        <v>422</v>
+      </c>
       <c r="H40" s="32"/>
       <c r="I40" s="32"/>
       <c r="J40" s="32"/>
@@ -44102,7 +44264,9 @@
       <c r="D41" s="32"/>
       <c r="E41" s="32"/>
       <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
+      <c r="G41" s="89" t="s">
+        <v>423</v>
+      </c>
       <c r="H41" s="32"/>
       <c r="I41" s="32"/>
       <c r="J41" s="32"/>
@@ -44115,7 +44279,9 @@
       <c r="D42" s="32"/>
       <c r="E42" s="32"/>
       <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
+      <c r="G42" s="89" t="s">
+        <v>428</v>
+      </c>
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
       <c r="J42" s="32"/>
@@ -44238,10 +44404,23 @@
       <c r="J51" s="32"/>
       <c r="K51" s="32"/>
     </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="32"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
+      <c r="J52" s="32"/>
+      <c r="K52" s="32"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:K51"/>
+  <autoFilter ref="B1:K52"/>
   <phoneticPr fontId="4"/>
-  <conditionalFormatting sqref="A2:K9 I24:K24 A36:K51 A10:F35 H25:K27 H19:K22 I10:K16 I18:K18 J17:K17 H29:K35 I28:K28 J23:K23">
+  <conditionalFormatting sqref="A2:K9 I24:K24 H25:K27 H19:K22 I10:K16 I18:K18 J17:K17 I28:K28 J23:K23 A38:K52 A10:F37 H29:K37">
     <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
       <formula>$D2="要望"</formula>
     </cfRule>
@@ -44285,7 +44464,7 @@
       <formula>$D26="対応"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G12:G17 G10">
+  <conditionalFormatting sqref="G12:G17 G10 G35">
     <cfRule type="expression" dxfId="5" priority="4834" stopIfTrue="1">
       <formula>$D12="要望"</formula>
     </cfRule>
@@ -44308,19 +44487,19 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I16 I29:I51 I18:I22 I24:I27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I16 I29:I52 I18:I22 I24:I27">
       <formula1>登録者</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B52">
       <formula1>重要度</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F52">
       <formula1>担当者</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D52">
       <formula1>状況</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E52">
       <formula1>状況２</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>